<commit_message>
updates to gantt chart
</commit_message>
<xml_diff>
--- a/docs/0b_forms/gantt_chart.xlsx
+++ b/docs/0b_forms/gantt_chart.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathantang/Documents/OneDrive - Goldsmiths College/Year-2/2-Software_Projects/repo/0b_forms/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathantang/Documents/OneDrive - Goldsmiths College/Year-2/2-Software_Projects/repo/docs/0b_forms/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="prevWBS" localSheetId="0">GanttChart!$A1048576</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">GanttChart!$A$1:$BN$66</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">GanttChart!$A$1:$BN$71</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">GanttChartPro!$A$1:$C$47</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">GanttChart!$4:$7</definedName>
     <definedName name="valuevx">42.314159</definedName>
@@ -121,7 +121,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="195">
   <si>
     <t>WBS</t>
   </si>
@@ -1325,6 +1325,24 @@
   </si>
   <si>
     <t>Preparation</t>
+  </si>
+  <si>
+    <t>Implementaiton</t>
+  </si>
+  <si>
+    <t>Testing Documentation</t>
+  </si>
+  <si>
+    <t>Tests</t>
+  </si>
+  <si>
+    <t>Bluetooth</t>
+  </si>
+  <si>
+    <t>AR Part 1</t>
+  </si>
+  <si>
+    <t>AR Part 2</t>
   </si>
 </sst>
 </file>
@@ -2700,24 +2718,6 @@
     <xf numFmtId="0" fontId="40" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="43" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="43" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="43" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2725,9 +2725,27 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="43" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="43" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="43" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="43" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2779,7 +2797,137 @@
     <cellStyle name="Total" xfId="42" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="43" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="66">
+  <dxfs count="81">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <border>
         <left style="thin">
@@ -3568,7 +3716,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$H$4" horiz="1" max="100" min="1" page="0" val="4"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$H$4" horiz="1" max="100" min="1" page="0" val="14"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3591,7 +3739,7 @@
         <xdr:cNvPr id="8236" name="Text Box 44" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002C200000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002C200000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3655,7 +3803,7 @@
                   <a14:compatExt spid="_x0000_s8238"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002E200000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002E200000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3705,7 +3853,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3789,7 +3937,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3844,7 +3992,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3899,7 +4047,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4224,11 +4372,11 @@
   <sheetPr codeName="Sheet8" enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BN73"/>
+  <dimension ref="A1:BN78"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H57" sqref="H57"/>
+      <pane ySplit="7" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4256,27 +4404,27 @@
       <c r="E1" s="47"/>
       <c r="F1" s="47"/>
       <c r="I1" s="126"/>
-      <c r="K1" s="179"/>
-      <c r="L1" s="179"/>
-      <c r="M1" s="179"/>
-      <c r="N1" s="179"/>
-      <c r="O1" s="179"/>
-      <c r="P1" s="179"/>
-      <c r="Q1" s="179"/>
-      <c r="R1" s="179"/>
-      <c r="S1" s="179"/>
-      <c r="T1" s="179"/>
-      <c r="U1" s="179"/>
-      <c r="V1" s="179"/>
-      <c r="W1" s="179"/>
-      <c r="X1" s="179"/>
-      <c r="Y1" s="179"/>
-      <c r="Z1" s="179"/>
-      <c r="AA1" s="179"/>
-      <c r="AB1" s="179"/>
-      <c r="AC1" s="179"/>
-      <c r="AD1" s="179"/>
-      <c r="AE1" s="179"/>
+      <c r="K1" s="173"/>
+      <c r="L1" s="173"/>
+      <c r="M1" s="173"/>
+      <c r="N1" s="173"/>
+      <c r="O1" s="173"/>
+      <c r="P1" s="173"/>
+      <c r="Q1" s="173"/>
+      <c r="R1" s="173"/>
+      <c r="S1" s="173"/>
+      <c r="T1" s="173"/>
+      <c r="U1" s="173"/>
+      <c r="V1" s="173"/>
+      <c r="W1" s="173"/>
+      <c r="X1" s="173"/>
+      <c r="Y1" s="173"/>
+      <c r="Z1" s="173"/>
+      <c r="AA1" s="173"/>
+      <c r="AB1" s="173"/>
+      <c r="AC1" s="173"/>
+      <c r="AD1" s="173"/>
+      <c r="AE1" s="173"/>
     </row>
     <row r="2" spans="1:66" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="52" t="s">
@@ -4321,196 +4469,196 @@
       <c r="B4" s="111" t="s">
         <v>74</v>
       </c>
-      <c r="C4" s="181">
+      <c r="C4" s="178">
         <v>43374</v>
       </c>
-      <c r="D4" s="181"/>
-      <c r="E4" s="181"/>
+      <c r="D4" s="178"/>
+      <c r="E4" s="178"/>
       <c r="F4" s="108"/>
       <c r="G4" s="111" t="s">
         <v>73</v>
       </c>
       <c r="H4" s="123">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="I4" s="109"/>
       <c r="J4" s="50"/>
-      <c r="K4" s="173" t="str">
+      <c r="K4" s="175" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 4</v>
-      </c>
-      <c r="L4" s="174"/>
-      <c r="M4" s="174"/>
-      <c r="N4" s="174"/>
-      <c r="O4" s="174"/>
-      <c r="P4" s="174"/>
-      <c r="Q4" s="175"/>
-      <c r="R4" s="173" t="str">
+        <v>Week 14</v>
+      </c>
+      <c r="L4" s="176"/>
+      <c r="M4" s="176"/>
+      <c r="N4" s="176"/>
+      <c r="O4" s="176"/>
+      <c r="P4" s="176"/>
+      <c r="Q4" s="177"/>
+      <c r="R4" s="175" t="str">
         <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 5</v>
-      </c>
-      <c r="S4" s="174"/>
-      <c r="T4" s="174"/>
-      <c r="U4" s="174"/>
-      <c r="V4" s="174"/>
-      <c r="W4" s="174"/>
-      <c r="X4" s="175"/>
-      <c r="Y4" s="173" t="str">
+        <v>Week 15</v>
+      </c>
+      <c r="S4" s="176"/>
+      <c r="T4" s="176"/>
+      <c r="U4" s="176"/>
+      <c r="V4" s="176"/>
+      <c r="W4" s="176"/>
+      <c r="X4" s="177"/>
+      <c r="Y4" s="175" t="str">
         <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 6</v>
-      </c>
-      <c r="Z4" s="174"/>
-      <c r="AA4" s="174"/>
-      <c r="AB4" s="174"/>
-      <c r="AC4" s="174"/>
-      <c r="AD4" s="174"/>
-      <c r="AE4" s="175"/>
-      <c r="AF4" s="173" t="str">
+        <v>Week 16</v>
+      </c>
+      <c r="Z4" s="176"/>
+      <c r="AA4" s="176"/>
+      <c r="AB4" s="176"/>
+      <c r="AC4" s="176"/>
+      <c r="AD4" s="176"/>
+      <c r="AE4" s="177"/>
+      <c r="AF4" s="175" t="str">
         <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 7</v>
-      </c>
-      <c r="AG4" s="174"/>
-      <c r="AH4" s="174"/>
-      <c r="AI4" s="174"/>
-      <c r="AJ4" s="174"/>
-      <c r="AK4" s="174"/>
-      <c r="AL4" s="175"/>
-      <c r="AM4" s="173" t="str">
+        <v>Week 17</v>
+      </c>
+      <c r="AG4" s="176"/>
+      <c r="AH4" s="176"/>
+      <c r="AI4" s="176"/>
+      <c r="AJ4" s="176"/>
+      <c r="AK4" s="176"/>
+      <c r="AL4" s="177"/>
+      <c r="AM4" s="175" t="str">
         <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 8</v>
-      </c>
-      <c r="AN4" s="174"/>
-      <c r="AO4" s="174"/>
-      <c r="AP4" s="174"/>
-      <c r="AQ4" s="174"/>
-      <c r="AR4" s="174"/>
-      <c r="AS4" s="175"/>
-      <c r="AT4" s="173" t="str">
+        <v>Week 18</v>
+      </c>
+      <c r="AN4" s="176"/>
+      <c r="AO4" s="176"/>
+      <c r="AP4" s="176"/>
+      <c r="AQ4" s="176"/>
+      <c r="AR4" s="176"/>
+      <c r="AS4" s="177"/>
+      <c r="AT4" s="175" t="str">
         <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 9</v>
-      </c>
-      <c r="AU4" s="174"/>
-      <c r="AV4" s="174"/>
-      <c r="AW4" s="174"/>
-      <c r="AX4" s="174"/>
-      <c r="AY4" s="174"/>
-      <c r="AZ4" s="175"/>
-      <c r="BA4" s="173" t="str">
+        <v>Week 19</v>
+      </c>
+      <c r="AU4" s="176"/>
+      <c r="AV4" s="176"/>
+      <c r="AW4" s="176"/>
+      <c r="AX4" s="176"/>
+      <c r="AY4" s="176"/>
+      <c r="AZ4" s="177"/>
+      <c r="BA4" s="175" t="str">
         <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 10</v>
-      </c>
-      <c r="BB4" s="174"/>
-      <c r="BC4" s="174"/>
-      <c r="BD4" s="174"/>
-      <c r="BE4" s="174"/>
-      <c r="BF4" s="174"/>
-      <c r="BG4" s="175"/>
-      <c r="BH4" s="173" t="str">
+        <v>Week 20</v>
+      </c>
+      <c r="BB4" s="176"/>
+      <c r="BC4" s="176"/>
+      <c r="BD4" s="176"/>
+      <c r="BE4" s="176"/>
+      <c r="BF4" s="176"/>
+      <c r="BG4" s="177"/>
+      <c r="BH4" s="175" t="str">
         <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 11</v>
-      </c>
-      <c r="BI4" s="174"/>
-      <c r="BJ4" s="174"/>
-      <c r="BK4" s="174"/>
-      <c r="BL4" s="174"/>
-      <c r="BM4" s="174"/>
-      <c r="BN4" s="175"/>
+        <v>Week 21</v>
+      </c>
+      <c r="BI4" s="176"/>
+      <c r="BJ4" s="176"/>
+      <c r="BK4" s="176"/>
+      <c r="BL4" s="176"/>
+      <c r="BM4" s="176"/>
+      <c r="BN4" s="177"/>
     </row>
     <row r="5" spans="1:66" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="107"/>
       <c r="B5" s="111" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="180">
+      <c r="C5" s="174">
         <v>43612</v>
       </c>
-      <c r="D5" s="180"/>
-      <c r="E5" s="180"/>
+      <c r="D5" s="174"/>
+      <c r="E5" s="174"/>
       <c r="F5" s="110"/>
       <c r="G5" s="110"/>
       <c r="H5" s="110"/>
       <c r="I5" s="110"/>
       <c r="J5" s="50"/>
-      <c r="K5" s="176">
+      <c r="K5" s="179">
         <f>K6</f>
-        <v>43395</v>
-      </c>
-      <c r="L5" s="177"/>
-      <c r="M5" s="177"/>
-      <c r="N5" s="177"/>
-      <c r="O5" s="177"/>
-      <c r="P5" s="177"/>
-      <c r="Q5" s="178"/>
-      <c r="R5" s="176">
+        <v>43465</v>
+      </c>
+      <c r="L5" s="180"/>
+      <c r="M5" s="180"/>
+      <c r="N5" s="180"/>
+      <c r="O5" s="180"/>
+      <c r="P5" s="180"/>
+      <c r="Q5" s="181"/>
+      <c r="R5" s="179">
         <f>R6</f>
-        <v>43402</v>
-      </c>
-      <c r="S5" s="177"/>
-      <c r="T5" s="177"/>
-      <c r="U5" s="177"/>
-      <c r="V5" s="177"/>
-      <c r="W5" s="177"/>
-      <c r="X5" s="178"/>
-      <c r="Y5" s="176">
+        <v>43472</v>
+      </c>
+      <c r="S5" s="180"/>
+      <c r="T5" s="180"/>
+      <c r="U5" s="180"/>
+      <c r="V5" s="180"/>
+      <c r="W5" s="180"/>
+      <c r="X5" s="181"/>
+      <c r="Y5" s="179">
         <f>Y6</f>
-        <v>43409</v>
-      </c>
-      <c r="Z5" s="177"/>
-      <c r="AA5" s="177"/>
-      <c r="AB5" s="177"/>
-      <c r="AC5" s="177"/>
-      <c r="AD5" s="177"/>
-      <c r="AE5" s="178"/>
-      <c r="AF5" s="176">
+        <v>43479</v>
+      </c>
+      <c r="Z5" s="180"/>
+      <c r="AA5" s="180"/>
+      <c r="AB5" s="180"/>
+      <c r="AC5" s="180"/>
+      <c r="AD5" s="180"/>
+      <c r="AE5" s="181"/>
+      <c r="AF5" s="179">
         <f>AF6</f>
-        <v>43416</v>
-      </c>
-      <c r="AG5" s="177"/>
-      <c r="AH5" s="177"/>
-      <c r="AI5" s="177"/>
-      <c r="AJ5" s="177"/>
-      <c r="AK5" s="177"/>
-      <c r="AL5" s="178"/>
-      <c r="AM5" s="176">
+        <v>43486</v>
+      </c>
+      <c r="AG5" s="180"/>
+      <c r="AH5" s="180"/>
+      <c r="AI5" s="180"/>
+      <c r="AJ5" s="180"/>
+      <c r="AK5" s="180"/>
+      <c r="AL5" s="181"/>
+      <c r="AM5" s="179">
         <f>AM6</f>
-        <v>43423</v>
-      </c>
-      <c r="AN5" s="177"/>
-      <c r="AO5" s="177"/>
-      <c r="AP5" s="177"/>
-      <c r="AQ5" s="177"/>
-      <c r="AR5" s="177"/>
-      <c r="AS5" s="178"/>
-      <c r="AT5" s="176">
+        <v>43493</v>
+      </c>
+      <c r="AN5" s="180"/>
+      <c r="AO5" s="180"/>
+      <c r="AP5" s="180"/>
+      <c r="AQ5" s="180"/>
+      <c r="AR5" s="180"/>
+      <c r="AS5" s="181"/>
+      <c r="AT5" s="179">
         <f>AT6</f>
-        <v>43430</v>
-      </c>
-      <c r="AU5" s="177"/>
-      <c r="AV5" s="177"/>
-      <c r="AW5" s="177"/>
-      <c r="AX5" s="177"/>
-      <c r="AY5" s="177"/>
-      <c r="AZ5" s="178"/>
-      <c r="BA5" s="176">
+        <v>43500</v>
+      </c>
+      <c r="AU5" s="180"/>
+      <c r="AV5" s="180"/>
+      <c r="AW5" s="180"/>
+      <c r="AX5" s="180"/>
+      <c r="AY5" s="180"/>
+      <c r="AZ5" s="181"/>
+      <c r="BA5" s="179">
         <f>BA6</f>
-        <v>43437</v>
-      </c>
-      <c r="BB5" s="177"/>
-      <c r="BC5" s="177"/>
-      <c r="BD5" s="177"/>
-      <c r="BE5" s="177"/>
-      <c r="BF5" s="177"/>
-      <c r="BG5" s="178"/>
-      <c r="BH5" s="176">
+        <v>43507</v>
+      </c>
+      <c r="BB5" s="180"/>
+      <c r="BC5" s="180"/>
+      <c r="BD5" s="180"/>
+      <c r="BE5" s="180"/>
+      <c r="BF5" s="180"/>
+      <c r="BG5" s="181"/>
+      <c r="BH5" s="179">
         <f>BH6</f>
-        <v>43444</v>
-      </c>
-      <c r="BI5" s="177"/>
-      <c r="BJ5" s="177"/>
-      <c r="BK5" s="177"/>
-      <c r="BL5" s="177"/>
-      <c r="BM5" s="177"/>
-      <c r="BN5" s="178"/>
+        <v>43514</v>
+      </c>
+      <c r="BI5" s="180"/>
+      <c r="BJ5" s="180"/>
+      <c r="BK5" s="180"/>
+      <c r="BL5" s="180"/>
+      <c r="BM5" s="180"/>
+      <c r="BN5" s="181"/>
     </row>
     <row r="6" spans="1:66" x14ac:dyDescent="0.15">
       <c r="A6" s="49"/>
@@ -4525,227 +4673,227 @@
       <c r="J6" s="50"/>
       <c r="K6" s="91">
         <f>C4-WEEKDAY(C4,1)+2+7*(H4-1)</f>
-        <v>43395</v>
+        <v>43465</v>
       </c>
       <c r="L6" s="83">
         <f t="shared" ref="L6:AQ6" si="0">K6+1</f>
-        <v>43396</v>
+        <v>43466</v>
       </c>
       <c r="M6" s="83">
         <f t="shared" si="0"/>
-        <v>43397</v>
+        <v>43467</v>
       </c>
       <c r="N6" s="83">
         <f t="shared" si="0"/>
-        <v>43398</v>
+        <v>43468</v>
       </c>
       <c r="O6" s="83">
         <f t="shared" si="0"/>
-        <v>43399</v>
+        <v>43469</v>
       </c>
       <c r="P6" s="83">
         <f t="shared" si="0"/>
-        <v>43400</v>
+        <v>43470</v>
       </c>
       <c r="Q6" s="92">
         <f t="shared" si="0"/>
-        <v>43401</v>
+        <v>43471</v>
       </c>
       <c r="R6" s="91">
         <f t="shared" si="0"/>
-        <v>43402</v>
+        <v>43472</v>
       </c>
       <c r="S6" s="83">
         <f t="shared" si="0"/>
-        <v>43403</v>
+        <v>43473</v>
       </c>
       <c r="T6" s="83">
         <f t="shared" si="0"/>
-        <v>43404</v>
+        <v>43474</v>
       </c>
       <c r="U6" s="83">
         <f t="shared" si="0"/>
-        <v>43405</v>
+        <v>43475</v>
       </c>
       <c r="V6" s="83">
         <f t="shared" si="0"/>
-        <v>43406</v>
+        <v>43476</v>
       </c>
       <c r="W6" s="83">
         <f t="shared" si="0"/>
-        <v>43407</v>
+        <v>43477</v>
       </c>
       <c r="X6" s="92">
         <f t="shared" si="0"/>
-        <v>43408</v>
+        <v>43478</v>
       </c>
       <c r="Y6" s="91">
         <f t="shared" si="0"/>
-        <v>43409</v>
+        <v>43479</v>
       </c>
       <c r="Z6" s="83">
         <f t="shared" si="0"/>
-        <v>43410</v>
+        <v>43480</v>
       </c>
       <c r="AA6" s="83">
         <f t="shared" si="0"/>
-        <v>43411</v>
+        <v>43481</v>
       </c>
       <c r="AB6" s="83">
         <f t="shared" si="0"/>
-        <v>43412</v>
+        <v>43482</v>
       </c>
       <c r="AC6" s="83">
         <f t="shared" si="0"/>
-        <v>43413</v>
+        <v>43483</v>
       </c>
       <c r="AD6" s="83">
         <f t="shared" si="0"/>
-        <v>43414</v>
+        <v>43484</v>
       </c>
       <c r="AE6" s="92">
         <f t="shared" si="0"/>
-        <v>43415</v>
+        <v>43485</v>
       </c>
       <c r="AF6" s="91">
         <f t="shared" si="0"/>
-        <v>43416</v>
+        <v>43486</v>
       </c>
       <c r="AG6" s="83">
         <f t="shared" si="0"/>
-        <v>43417</v>
+        <v>43487</v>
       </c>
       <c r="AH6" s="83">
         <f t="shared" si="0"/>
-        <v>43418</v>
+        <v>43488</v>
       </c>
       <c r="AI6" s="83">
         <f t="shared" si="0"/>
-        <v>43419</v>
+        <v>43489</v>
       </c>
       <c r="AJ6" s="83">
         <f t="shared" si="0"/>
-        <v>43420</v>
+        <v>43490</v>
       </c>
       <c r="AK6" s="83">
         <f t="shared" si="0"/>
-        <v>43421</v>
+        <v>43491</v>
       </c>
       <c r="AL6" s="92">
         <f t="shared" si="0"/>
-        <v>43422</v>
+        <v>43492</v>
       </c>
       <c r="AM6" s="91">
         <f t="shared" si="0"/>
-        <v>43423</v>
+        <v>43493</v>
       </c>
       <c r="AN6" s="83">
         <f t="shared" si="0"/>
-        <v>43424</v>
+        <v>43494</v>
       </c>
       <c r="AO6" s="83">
         <f t="shared" si="0"/>
-        <v>43425</v>
+        <v>43495</v>
       </c>
       <c r="AP6" s="83">
         <f t="shared" si="0"/>
-        <v>43426</v>
+        <v>43496</v>
       </c>
       <c r="AQ6" s="83">
         <f t="shared" si="0"/>
-        <v>43427</v>
+        <v>43497</v>
       </c>
       <c r="AR6" s="83">
         <f t="shared" ref="AR6:BN6" si="1">AQ6+1</f>
-        <v>43428</v>
+        <v>43498</v>
       </c>
       <c r="AS6" s="92">
         <f t="shared" si="1"/>
-        <v>43429</v>
+        <v>43499</v>
       </c>
       <c r="AT6" s="91">
         <f t="shared" si="1"/>
-        <v>43430</v>
+        <v>43500</v>
       </c>
       <c r="AU6" s="83">
         <f t="shared" si="1"/>
-        <v>43431</v>
+        <v>43501</v>
       </c>
       <c r="AV6" s="83">
         <f t="shared" si="1"/>
-        <v>43432</v>
+        <v>43502</v>
       </c>
       <c r="AW6" s="83">
         <f t="shared" si="1"/>
-        <v>43433</v>
+        <v>43503</v>
       </c>
       <c r="AX6" s="83">
         <f t="shared" si="1"/>
-        <v>43434</v>
+        <v>43504</v>
       </c>
       <c r="AY6" s="83">
         <f t="shared" si="1"/>
-        <v>43435</v>
+        <v>43505</v>
       </c>
       <c r="AZ6" s="92">
         <f t="shared" si="1"/>
-        <v>43436</v>
+        <v>43506</v>
       </c>
       <c r="BA6" s="91">
         <f t="shared" si="1"/>
-        <v>43437</v>
+        <v>43507</v>
       </c>
       <c r="BB6" s="83">
         <f t="shared" si="1"/>
-        <v>43438</v>
+        <v>43508</v>
       </c>
       <c r="BC6" s="83">
         <f t="shared" si="1"/>
-        <v>43439</v>
+        <v>43509</v>
       </c>
       <c r="BD6" s="83">
         <f t="shared" si="1"/>
-        <v>43440</v>
+        <v>43510</v>
       </c>
       <c r="BE6" s="83">
         <f t="shared" si="1"/>
-        <v>43441</v>
+        <v>43511</v>
       </c>
       <c r="BF6" s="83">
         <f t="shared" si="1"/>
-        <v>43442</v>
+        <v>43512</v>
       </c>
       <c r="BG6" s="92">
         <f t="shared" si="1"/>
-        <v>43443</v>
+        <v>43513</v>
       </c>
       <c r="BH6" s="91">
         <f t="shared" si="1"/>
-        <v>43444</v>
+        <v>43514</v>
       </c>
       <c r="BI6" s="83">
         <f t="shared" si="1"/>
-        <v>43445</v>
+        <v>43515</v>
       </c>
       <c r="BJ6" s="83">
         <f t="shared" si="1"/>
-        <v>43446</v>
+        <v>43516</v>
       </c>
       <c r="BK6" s="83">
         <f t="shared" si="1"/>
-        <v>43447</v>
+        <v>43517</v>
       </c>
       <c r="BL6" s="83">
         <f t="shared" si="1"/>
-        <v>43448</v>
+        <v>43518</v>
       </c>
       <c r="BM6" s="83">
         <f t="shared" si="1"/>
-        <v>43449</v>
+        <v>43519</v>
       </c>
       <c r="BN6" s="92">
         <f t="shared" si="1"/>
-        <v>43450</v>
+        <v>43520</v>
       </c>
     </row>
     <row r="7" spans="1:66" s="157" customFormat="1" ht="25" thickBot="1" x14ac:dyDescent="0.2">
@@ -5020,7 +5168,7 @@
       <c r="G8" s="88"/>
       <c r="H8" s="89"/>
       <c r="I8" s="90" t="str">
-        <f t="shared" ref="I8:I66" si="4">IF(OR(F8=0,E8=0)," - ",NETWORKDAYS(E8,F8))</f>
+        <f t="shared" ref="I8:I71" si="4">IF(OR(F8=0,E8=0)," - ",NETWORKDAYS(E8,F8))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J8" s="93"/>
@@ -7928,7 +8076,7 @@
         <v>43388</v>
       </c>
       <c r="F43" s="163">
-        <f t="shared" ref="F43:F63" si="28">IF(ISBLANK(E43)," - ",IF(G43=0,E43,E43+G43-1))</f>
+        <f t="shared" ref="F43:F68" si="28">IF(ISBLANK(E43)," - ",IF(G43=0,E43,E43+G43-1))</f>
         <v>43391</v>
       </c>
       <c r="G43" s="62">
@@ -7938,7 +8086,7 @@
         <v>1</v>
       </c>
       <c r="I43" s="80">
-        <f t="shared" ref="I43:I63" si="29">IF(OR(F43=0,E43=0)," - ",NETWORKDAYS(E43,F43))</f>
+        <f t="shared" ref="I43:I68" si="29">IF(OR(F43=0,E43=0)," - ",NETWORKDAYS(E43,F43))</f>
         <v>4</v>
       </c>
       <c r="J43" s="98"/>
@@ -9094,19 +9242,27 @@
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>9.1</v>
       </c>
-      <c r="B57" s="81"/>
+      <c r="B57" s="81" t="s">
+        <v>190</v>
+      </c>
       <c r="C57" s="81"/>
       <c r="D57" s="79"/>
-      <c r="E57" s="160"/>
-      <c r="F57" s="163" t="str">
+      <c r="E57" s="160">
+        <v>43479</v>
+      </c>
+      <c r="F57" s="163">
         <f>IF(ISBLANK(E57)," - ",IF(G57=0,E57,E57+G57-1))</f>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="G57" s="62"/>
-      <c r="H57" s="63"/>
-      <c r="I57" s="80" t="str">
+        <v>43490</v>
+      </c>
+      <c r="G57" s="62">
+        <v>12</v>
+      </c>
+      <c r="H57" s="63">
+        <v>0.8</v>
+      </c>
+      <c r="I57" s="80">
         <f>IF(OR(F57=0,E57=0)," - ",NETWORKDAYS(E57,F57))</f>
-        <v xml:space="preserve"> - </v>
+        <v>10</v>
       </c>
       <c r="J57" s="98"/>
       <c r="K57" s="105"/>
@@ -9166,257 +9322,276 @@
       <c r="BM57" s="105"/>
       <c r="BN57" s="105"/>
     </row>
-    <row r="58" spans="1:66" s="55" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A58" s="53" t="str">
+    <row r="58" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.15">
+      <c r="A58" s="60" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>9.2</v>
+      </c>
+      <c r="B58" s="81" t="s">
+        <v>191</v>
+      </c>
+      <c r="C58" s="81"/>
+      <c r="D58" s="79"/>
+      <c r="E58" s="160">
+        <v>43479</v>
+      </c>
+      <c r="F58" s="163">
+        <f>IF(ISBLANK(E58)," - ",IF(G58=0,E58,E58+G58-1))</f>
+        <v>43490</v>
+      </c>
+      <c r="G58" s="62">
+        <v>12</v>
+      </c>
+      <c r="H58" s="63">
+        <v>0.5</v>
+      </c>
+      <c r="I58" s="80">
+        <f>IF(OR(F58=0,E58=0)," - ",NETWORKDAYS(E58,F58))</f>
+        <v>10</v>
+      </c>
+      <c r="J58" s="98"/>
+      <c r="K58" s="105"/>
+      <c r="L58" s="105"/>
+      <c r="M58" s="105"/>
+      <c r="N58" s="105"/>
+      <c r="O58" s="105"/>
+      <c r="P58" s="105"/>
+      <c r="Q58" s="105"/>
+      <c r="R58" s="105"/>
+      <c r="S58" s="105"/>
+      <c r="T58" s="105"/>
+      <c r="U58" s="105"/>
+      <c r="V58" s="105"/>
+      <c r="W58" s="105"/>
+      <c r="X58" s="105"/>
+      <c r="Y58" s="105"/>
+      <c r="Z58" s="105"/>
+      <c r="AA58" s="105"/>
+      <c r="AB58" s="105"/>
+      <c r="AC58" s="105"/>
+      <c r="AD58" s="105"/>
+      <c r="AE58" s="105"/>
+      <c r="AF58" s="105"/>
+      <c r="AG58" s="105"/>
+      <c r="AH58" s="105"/>
+      <c r="AI58" s="105"/>
+      <c r="AJ58" s="105"/>
+      <c r="AK58" s="105"/>
+      <c r="AL58" s="105"/>
+      <c r="AM58" s="105"/>
+      <c r="AN58" s="105"/>
+      <c r="AO58" s="105"/>
+      <c r="AP58" s="105"/>
+      <c r="AQ58" s="105"/>
+      <c r="AR58" s="105"/>
+      <c r="AS58" s="105"/>
+      <c r="AT58" s="105"/>
+      <c r="AU58" s="105"/>
+      <c r="AV58" s="105"/>
+      <c r="AW58" s="105"/>
+      <c r="AX58" s="105"/>
+      <c r="AY58" s="105"/>
+      <c r="AZ58" s="105"/>
+      <c r="BA58" s="105"/>
+      <c r="BB58" s="105"/>
+      <c r="BC58" s="105"/>
+      <c r="BD58" s="105"/>
+      <c r="BE58" s="105"/>
+      <c r="BF58" s="105"/>
+      <c r="BG58" s="105"/>
+      <c r="BH58" s="105"/>
+      <c r="BI58" s="105"/>
+      <c r="BJ58" s="105"/>
+      <c r="BK58" s="105"/>
+      <c r="BL58" s="105"/>
+      <c r="BM58" s="105"/>
+      <c r="BN58" s="105"/>
+    </row>
+    <row r="59" spans="1:66" s="55" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A59" s="53" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>10</v>
       </c>
-      <c r="B58" s="54" t="s">
-        <v>153</v>
-      </c>
-      <c r="D58" s="56"/>
-      <c r="E58" s="161"/>
-      <c r="F58" s="161" t="str">
-        <f t="shared" ref="F58:F59" si="34">IF(ISBLANK(E58)," - ",IF(G58=0,E58,E58+G58-1))</f>
+      <c r="B59" s="54" t="s">
+        <v>189</v>
+      </c>
+      <c r="D59" s="56"/>
+      <c r="E59" s="161"/>
+      <c r="F59" s="161" t="str">
+        <f t="shared" ref="F59" si="34">IF(ISBLANK(E59)," - ",IF(G59=0,E59,E59+G59-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="G58" s="57"/>
-      <c r="H58" s="58"/>
-      <c r="I58" s="59" t="str">
-        <f t="shared" ref="I58:I59" si="35">IF(OR(F58=0,E58=0)," - ",NETWORKDAYS(E58,F58))</f>
+      <c r="G59" s="57"/>
+      <c r="H59" s="58"/>
+      <c r="I59" s="59" t="str">
+        <f t="shared" ref="I59" si="35">IF(OR(F59=0,E59=0)," - ",NETWORKDAYS(E59,F59))</f>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="J58" s="95"/>
-      <c r="K58" s="106"/>
-      <c r="L58" s="106"/>
-      <c r="M58" s="106"/>
-      <c r="N58" s="106"/>
-      <c r="O58" s="106"/>
-      <c r="P58" s="106"/>
-      <c r="Q58" s="106"/>
-      <c r="R58" s="106"/>
-      <c r="S58" s="106"/>
-      <c r="T58" s="106"/>
-      <c r="U58" s="106"/>
-      <c r="V58" s="106"/>
-      <c r="W58" s="106"/>
-      <c r="X58" s="106"/>
-      <c r="Y58" s="106"/>
-      <c r="Z58" s="106"/>
-      <c r="AA58" s="106"/>
-      <c r="AB58" s="106"/>
-      <c r="AC58" s="106"/>
-      <c r="AD58" s="106"/>
-      <c r="AE58" s="106"/>
-      <c r="AF58" s="106"/>
-      <c r="AG58" s="106"/>
-      <c r="AH58" s="106"/>
-      <c r="AI58" s="106"/>
-      <c r="AJ58" s="106"/>
-      <c r="AK58" s="106"/>
-      <c r="AL58" s="106"/>
-      <c r="AM58" s="106"/>
-      <c r="AN58" s="106"/>
-      <c r="AO58" s="106"/>
-      <c r="AP58" s="106"/>
-      <c r="AQ58" s="106"/>
-      <c r="AR58" s="106"/>
-      <c r="AS58" s="106"/>
-      <c r="AT58" s="106"/>
-      <c r="AU58" s="106"/>
-      <c r="AV58" s="106"/>
-      <c r="AW58" s="106"/>
-      <c r="AX58" s="106"/>
-      <c r="AY58" s="106"/>
-      <c r="AZ58" s="106"/>
-      <c r="BA58" s="106"/>
-      <c r="BB58" s="106"/>
-      <c r="BC58" s="106"/>
-      <c r="BD58" s="106"/>
-      <c r="BE58" s="106"/>
-      <c r="BF58" s="106"/>
-      <c r="BG58" s="106"/>
-      <c r="BH58" s="106"/>
-      <c r="BI58" s="106"/>
-      <c r="BJ58" s="106"/>
-      <c r="BK58" s="106"/>
-      <c r="BL58" s="106"/>
-      <c r="BM58" s="106"/>
-      <c r="BN58" s="106"/>
-    </row>
-    <row r="59" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A59" s="60" t="str">
+      <c r="J59" s="95"/>
+      <c r="K59" s="106"/>
+      <c r="L59" s="106"/>
+      <c r="M59" s="106"/>
+      <c r="N59" s="106"/>
+      <c r="O59" s="106"/>
+      <c r="P59" s="106"/>
+      <c r="Q59" s="106"/>
+      <c r="R59" s="106"/>
+      <c r="S59" s="106"/>
+      <c r="T59" s="106"/>
+      <c r="U59" s="106"/>
+      <c r="V59" s="106"/>
+      <c r="W59" s="106"/>
+      <c r="X59" s="106"/>
+      <c r="Y59" s="106"/>
+      <c r="Z59" s="106"/>
+      <c r="AA59" s="106"/>
+      <c r="AB59" s="106"/>
+      <c r="AC59" s="106"/>
+      <c r="AD59" s="106"/>
+      <c r="AE59" s="106"/>
+      <c r="AF59" s="106"/>
+      <c r="AG59" s="106"/>
+      <c r="AH59" s="106"/>
+      <c r="AI59" s="106"/>
+      <c r="AJ59" s="106"/>
+      <c r="AK59" s="106"/>
+      <c r="AL59" s="106"/>
+      <c r="AM59" s="106"/>
+      <c r="AN59" s="106"/>
+      <c r="AO59" s="106"/>
+      <c r="AP59" s="106"/>
+      <c r="AQ59" s="106"/>
+      <c r="AR59" s="106"/>
+      <c r="AS59" s="106"/>
+      <c r="AT59" s="106"/>
+      <c r="AU59" s="106"/>
+      <c r="AV59" s="106"/>
+      <c r="AW59" s="106"/>
+      <c r="AX59" s="106"/>
+      <c r="AY59" s="106"/>
+      <c r="AZ59" s="106"/>
+      <c r="BA59" s="106"/>
+      <c r="BB59" s="106"/>
+      <c r="BC59" s="106"/>
+      <c r="BD59" s="106"/>
+      <c r="BE59" s="106"/>
+      <c r="BF59" s="106"/>
+      <c r="BG59" s="106"/>
+      <c r="BH59" s="106"/>
+      <c r="BI59" s="106"/>
+      <c r="BJ59" s="106"/>
+      <c r="BK59" s="106"/>
+      <c r="BL59" s="106"/>
+      <c r="BM59" s="106"/>
+      <c r="BN59" s="106"/>
+    </row>
+    <row r="60" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.15">
+      <c r="A60" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>10.1</v>
       </c>
-      <c r="B59" s="81"/>
-      <c r="C59" s="81"/>
-      <c r="D59" s="79"/>
-      <c r="E59" s="160"/>
-      <c r="F59" s="163" t="str">
-        <f t="shared" si="34"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="G59" s="62"/>
-      <c r="H59" s="63"/>
-      <c r="I59" s="80" t="str">
-        <f t="shared" si="35"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J59" s="98"/>
-      <c r="K59" s="105"/>
-      <c r="L59" s="105"/>
-      <c r="M59" s="105"/>
-      <c r="N59" s="105"/>
-      <c r="O59" s="105"/>
-      <c r="P59" s="105"/>
-      <c r="Q59" s="105"/>
-      <c r="R59" s="105"/>
-      <c r="S59" s="105"/>
-      <c r="T59" s="105"/>
-      <c r="U59" s="105"/>
-      <c r="V59" s="105"/>
-      <c r="W59" s="105"/>
-      <c r="X59" s="105"/>
-      <c r="Y59" s="105"/>
-      <c r="Z59" s="105"/>
-      <c r="AA59" s="105"/>
-      <c r="AB59" s="105"/>
-      <c r="AC59" s="105"/>
-      <c r="AD59" s="105"/>
-      <c r="AE59" s="105"/>
-      <c r="AF59" s="105"/>
-      <c r="AG59" s="105"/>
-      <c r="AH59" s="105"/>
-      <c r="AI59" s="105"/>
-      <c r="AJ59" s="105"/>
-      <c r="AK59" s="105"/>
-      <c r="AL59" s="105"/>
-      <c r="AM59" s="105"/>
-      <c r="AN59" s="105"/>
-      <c r="AO59" s="105"/>
-      <c r="AP59" s="105"/>
-      <c r="AQ59" s="105"/>
-      <c r="AR59" s="105"/>
-      <c r="AS59" s="105"/>
-      <c r="AT59" s="105"/>
-      <c r="AU59" s="105"/>
-      <c r="AV59" s="105"/>
-      <c r="AW59" s="105"/>
-      <c r="AX59" s="105"/>
-      <c r="AY59" s="105"/>
-      <c r="AZ59" s="105"/>
-      <c r="BA59" s="105"/>
-      <c r="BB59" s="105"/>
-      <c r="BC59" s="105"/>
-      <c r="BD59" s="105"/>
-      <c r="BE59" s="105"/>
-      <c r="BF59" s="105"/>
-      <c r="BG59" s="105"/>
-      <c r="BH59" s="105"/>
-      <c r="BI59" s="105"/>
-      <c r="BJ59" s="105"/>
-      <c r="BK59" s="105"/>
-      <c r="BL59" s="105"/>
-      <c r="BM59" s="105"/>
-      <c r="BN59" s="105"/>
-    </row>
-    <row r="60" spans="1:66" s="55" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A60" s="53" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
-        <v>11</v>
-      </c>
-      <c r="B60" s="54" t="s">
-        <v>154</v>
-      </c>
-      <c r="D60" s="56"/>
-      <c r="E60" s="161"/>
-      <c r="F60" s="161" t="str">
-        <f t="shared" si="28"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="G60" s="57"/>
-      <c r="H60" s="58"/>
-      <c r="I60" s="59" t="str">
-        <f t="shared" si="29"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J60" s="95"/>
-      <c r="K60" s="106"/>
-      <c r="L60" s="106"/>
-      <c r="M60" s="106"/>
-      <c r="N60" s="106"/>
-      <c r="O60" s="106"/>
-      <c r="P60" s="106"/>
-      <c r="Q60" s="106"/>
-      <c r="R60" s="106"/>
-      <c r="S60" s="106"/>
-      <c r="T60" s="106"/>
-      <c r="U60" s="106"/>
-      <c r="V60" s="106"/>
-      <c r="W60" s="106"/>
-      <c r="X60" s="106"/>
-      <c r="Y60" s="106"/>
-      <c r="Z60" s="106"/>
-      <c r="AA60" s="106"/>
-      <c r="AB60" s="106"/>
-      <c r="AC60" s="106"/>
-      <c r="AD60" s="106"/>
-      <c r="AE60" s="106"/>
-      <c r="AF60" s="106"/>
-      <c r="AG60" s="106"/>
-      <c r="AH60" s="106"/>
-      <c r="AI60" s="106"/>
-      <c r="AJ60" s="106"/>
-      <c r="AK60" s="106"/>
-      <c r="AL60" s="106"/>
-      <c r="AM60" s="106"/>
-      <c r="AN60" s="106"/>
-      <c r="AO60" s="106"/>
-      <c r="AP60" s="106"/>
-      <c r="AQ60" s="106"/>
-      <c r="AR60" s="106"/>
-      <c r="AS60" s="106"/>
-      <c r="AT60" s="106"/>
-      <c r="AU60" s="106"/>
-      <c r="AV60" s="106"/>
-      <c r="AW60" s="106"/>
-      <c r="AX60" s="106"/>
-      <c r="AY60" s="106"/>
-      <c r="AZ60" s="106"/>
-      <c r="BA60" s="106"/>
-      <c r="BB60" s="106"/>
-      <c r="BC60" s="106"/>
-      <c r="BD60" s="106"/>
-      <c r="BE60" s="106"/>
-      <c r="BF60" s="106"/>
-      <c r="BG60" s="106"/>
-      <c r="BH60" s="106"/>
-      <c r="BI60" s="106"/>
-      <c r="BJ60" s="106"/>
-      <c r="BK60" s="106"/>
-      <c r="BL60" s="106"/>
-      <c r="BM60" s="106"/>
-      <c r="BN60" s="106"/>
+      <c r="B60" s="81" t="s">
+        <v>192</v>
+      </c>
+      <c r="C60" s="81"/>
+      <c r="D60" s="79"/>
+      <c r="E60" s="160">
+        <v>43484</v>
+      </c>
+      <c r="F60" s="163">
+        <f>IF(ISBLANK(E60)," - ",IF(G60=0,E60,E60+G60-1))</f>
+        <v>43499</v>
+      </c>
+      <c r="G60" s="62">
+        <v>16</v>
+      </c>
+      <c r="H60" s="63"/>
+      <c r="I60" s="80">
+        <f>IF(OR(F60=0,E60=0)," - ",NETWORKDAYS(E60,F60))</f>
+        <v>10</v>
+      </c>
+      <c r="J60" s="98"/>
+      <c r="K60" s="105"/>
+      <c r="L60" s="105"/>
+      <c r="M60" s="105"/>
+      <c r="N60" s="105"/>
+      <c r="O60" s="105"/>
+      <c r="P60" s="105"/>
+      <c r="Q60" s="105"/>
+      <c r="R60" s="105"/>
+      <c r="S60" s="105"/>
+      <c r="T60" s="105"/>
+      <c r="U60" s="105"/>
+      <c r="V60" s="105"/>
+      <c r="W60" s="105"/>
+      <c r="X60" s="105"/>
+      <c r="Y60" s="105"/>
+      <c r="Z60" s="105"/>
+      <c r="AA60" s="105"/>
+      <c r="AB60" s="105"/>
+      <c r="AC60" s="105"/>
+      <c r="AD60" s="105"/>
+      <c r="AE60" s="105"/>
+      <c r="AF60" s="105"/>
+      <c r="AG60" s="105"/>
+      <c r="AH60" s="105"/>
+      <c r="AI60" s="105"/>
+      <c r="AJ60" s="105"/>
+      <c r="AK60" s="105"/>
+      <c r="AL60" s="105"/>
+      <c r="AM60" s="105"/>
+      <c r="AN60" s="105"/>
+      <c r="AO60" s="105"/>
+      <c r="AP60" s="105"/>
+      <c r="AQ60" s="105"/>
+      <c r="AR60" s="105"/>
+      <c r="AS60" s="105"/>
+      <c r="AT60" s="105"/>
+      <c r="AU60" s="105"/>
+      <c r="AV60" s="105"/>
+      <c r="AW60" s="105"/>
+      <c r="AX60" s="105"/>
+      <c r="AY60" s="105"/>
+      <c r="AZ60" s="105"/>
+      <c r="BA60" s="105"/>
+      <c r="BB60" s="105"/>
+      <c r="BC60" s="105"/>
+      <c r="BD60" s="105"/>
+      <c r="BE60" s="105"/>
+      <c r="BF60" s="105"/>
+      <c r="BG60" s="105"/>
+      <c r="BH60" s="105"/>
+      <c r="BI60" s="105"/>
+      <c r="BJ60" s="105"/>
+      <c r="BK60" s="105"/>
+      <c r="BL60" s="105"/>
+      <c r="BM60" s="105"/>
+      <c r="BN60" s="105"/>
     </row>
     <row r="61" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.15">
       <c r="A61" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>11.1</v>
-      </c>
-      <c r="B61" s="81"/>
+        <v>10.2</v>
+      </c>
+      <c r="B61" s="81" t="s">
+        <v>193</v>
+      </c>
       <c r="C61" s="81"/>
       <c r="D61" s="79"/>
-      <c r="E61" s="160"/>
-      <c r="F61" s="163" t="str">
-        <f t="shared" si="28"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="G61" s="62"/>
+      <c r="E61" s="160">
+        <v>43500</v>
+      </c>
+      <c r="F61" s="163">
+        <f>IF(ISBLANK(E61)," - ",IF(G61=0,E61,E61+G61-1))</f>
+        <v>43513</v>
+      </c>
+      <c r="G61" s="62">
+        <v>14</v>
+      </c>
       <c r="H61" s="63"/>
-      <c r="I61" s="80" t="str">
-        <f t="shared" si="29"/>
-        <v xml:space="preserve"> - </v>
+      <c r="I61" s="80">
+        <f>IF(OR(F61=0,E61=0)," - ",NETWORKDAYS(E61,F61))</f>
+        <v>10</v>
       </c>
       <c r="J61" s="98"/>
       <c r="K61" s="105"/>
@@ -9476,330 +9651,342 @@
       <c r="BM61" s="105"/>
       <c r="BN61" s="105"/>
     </row>
-    <row r="62" spans="1:66" s="55" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A62" s="53" t="str">
+    <row r="62" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.15">
+      <c r="A62" s="60" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>10.3</v>
+      </c>
+      <c r="B62" s="81" t="s">
+        <v>194</v>
+      </c>
+      <c r="C62" s="81"/>
+      <c r="D62" s="79"/>
+      <c r="E62" s="160">
+        <v>43514</v>
+      </c>
+      <c r="F62" s="163">
+        <f>IF(ISBLANK(E62)," - ",IF(G62=0,E62,E62+G62-1))</f>
+        <v>43527</v>
+      </c>
+      <c r="G62" s="62">
+        <v>14</v>
+      </c>
+      <c r="H62" s="63"/>
+      <c r="I62" s="80">
+        <f>IF(OR(F62=0,E62=0)," - ",NETWORKDAYS(E62,F62))</f>
+        <v>10</v>
+      </c>
+      <c r="J62" s="98"/>
+      <c r="K62" s="105"/>
+      <c r="L62" s="105"/>
+      <c r="M62" s="105"/>
+      <c r="N62" s="105"/>
+      <c r="O62" s="105"/>
+      <c r="P62" s="105"/>
+      <c r="Q62" s="105"/>
+      <c r="R62" s="105"/>
+      <c r="S62" s="105"/>
+      <c r="T62" s="105"/>
+      <c r="U62" s="105"/>
+      <c r="V62" s="105"/>
+      <c r="W62" s="105"/>
+      <c r="X62" s="105"/>
+      <c r="Y62" s="105"/>
+      <c r="Z62" s="105"/>
+      <c r="AA62" s="105"/>
+      <c r="AB62" s="105"/>
+      <c r="AC62" s="105"/>
+      <c r="AD62" s="105"/>
+      <c r="AE62" s="105"/>
+      <c r="AF62" s="105"/>
+      <c r="AG62" s="105"/>
+      <c r="AH62" s="105"/>
+      <c r="AI62" s="105"/>
+      <c r="AJ62" s="105"/>
+      <c r="AK62" s="105"/>
+      <c r="AL62" s="105"/>
+      <c r="AM62" s="105"/>
+      <c r="AN62" s="105"/>
+      <c r="AO62" s="105"/>
+      <c r="AP62" s="105"/>
+      <c r="AQ62" s="105"/>
+      <c r="AR62" s="105"/>
+      <c r="AS62" s="105"/>
+      <c r="AT62" s="105"/>
+      <c r="AU62" s="105"/>
+      <c r="AV62" s="105"/>
+      <c r="AW62" s="105"/>
+      <c r="AX62" s="105"/>
+      <c r="AY62" s="105"/>
+      <c r="AZ62" s="105"/>
+      <c r="BA62" s="105"/>
+      <c r="BB62" s="105"/>
+      <c r="BC62" s="105"/>
+      <c r="BD62" s="105"/>
+      <c r="BE62" s="105"/>
+      <c r="BF62" s="105"/>
+      <c r="BG62" s="105"/>
+      <c r="BH62" s="105"/>
+      <c r="BI62" s="105"/>
+      <c r="BJ62" s="105"/>
+      <c r="BK62" s="105"/>
+      <c r="BL62" s="105"/>
+      <c r="BM62" s="105"/>
+      <c r="BN62" s="105"/>
+    </row>
+    <row r="63" spans="1:66" s="55" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A63" s="53" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+        <v>11</v>
+      </c>
+      <c r="B63" s="54" t="s">
+        <v>153</v>
+      </c>
+      <c r="D63" s="56"/>
+      <c r="E63" s="161"/>
+      <c r="F63" s="161" t="str">
+        <f t="shared" ref="F63:F64" si="36">IF(ISBLANK(E63)," - ",IF(G63=0,E63,E63+G63-1))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="G63" s="57"/>
+      <c r="H63" s="58"/>
+      <c r="I63" s="59" t="str">
+        <f t="shared" ref="I63:I64" si="37">IF(OR(F63=0,E63=0)," - ",NETWORKDAYS(E63,F63))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J63" s="95"/>
+      <c r="K63" s="106"/>
+      <c r="L63" s="106"/>
+      <c r="M63" s="106"/>
+      <c r="N63" s="106"/>
+      <c r="O63" s="106"/>
+      <c r="P63" s="106"/>
+      <c r="Q63" s="106"/>
+      <c r="R63" s="106"/>
+      <c r="S63" s="106"/>
+      <c r="T63" s="106"/>
+      <c r="U63" s="106"/>
+      <c r="V63" s="106"/>
+      <c r="W63" s="106"/>
+      <c r="X63" s="106"/>
+      <c r="Y63" s="106"/>
+      <c r="Z63" s="106"/>
+      <c r="AA63" s="106"/>
+      <c r="AB63" s="106"/>
+      <c r="AC63" s="106"/>
+      <c r="AD63" s="106"/>
+      <c r="AE63" s="106"/>
+      <c r="AF63" s="106"/>
+      <c r="AG63" s="106"/>
+      <c r="AH63" s="106"/>
+      <c r="AI63" s="106"/>
+      <c r="AJ63" s="106"/>
+      <c r="AK63" s="106"/>
+      <c r="AL63" s="106"/>
+      <c r="AM63" s="106"/>
+      <c r="AN63" s="106"/>
+      <c r="AO63" s="106"/>
+      <c r="AP63" s="106"/>
+      <c r="AQ63" s="106"/>
+      <c r="AR63" s="106"/>
+      <c r="AS63" s="106"/>
+      <c r="AT63" s="106"/>
+      <c r="AU63" s="106"/>
+      <c r="AV63" s="106"/>
+      <c r="AW63" s="106"/>
+      <c r="AX63" s="106"/>
+      <c r="AY63" s="106"/>
+      <c r="AZ63" s="106"/>
+      <c r="BA63" s="106"/>
+      <c r="BB63" s="106"/>
+      <c r="BC63" s="106"/>
+      <c r="BD63" s="106"/>
+      <c r="BE63" s="106"/>
+      <c r="BF63" s="106"/>
+      <c r="BG63" s="106"/>
+      <c r="BH63" s="106"/>
+      <c r="BI63" s="106"/>
+      <c r="BJ63" s="106"/>
+      <c r="BK63" s="106"/>
+      <c r="BL63" s="106"/>
+      <c r="BM63" s="106"/>
+      <c r="BN63" s="106"/>
+    </row>
+    <row r="64" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.15">
+      <c r="A64" s="60" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>11.1</v>
+      </c>
+      <c r="B64" s="81"/>
+      <c r="C64" s="81"/>
+      <c r="D64" s="79"/>
+      <c r="E64" s="160"/>
+      <c r="F64" s="163" t="str">
+        <f t="shared" si="36"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="G64" s="62"/>
+      <c r="H64" s="63"/>
+      <c r="I64" s="80" t="str">
+        <f t="shared" si="37"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J64" s="98"/>
+      <c r="K64" s="105"/>
+      <c r="L64" s="105"/>
+      <c r="M64" s="105"/>
+      <c r="N64" s="105"/>
+      <c r="O64" s="105"/>
+      <c r="P64" s="105"/>
+      <c r="Q64" s="105"/>
+      <c r="R64" s="105"/>
+      <c r="S64" s="105"/>
+      <c r="T64" s="105"/>
+      <c r="U64" s="105"/>
+      <c r="V64" s="105"/>
+      <c r="W64" s="105"/>
+      <c r="X64" s="105"/>
+      <c r="Y64" s="105"/>
+      <c r="Z64" s="105"/>
+      <c r="AA64" s="105"/>
+      <c r="AB64" s="105"/>
+      <c r="AC64" s="105"/>
+      <c r="AD64" s="105"/>
+      <c r="AE64" s="105"/>
+      <c r="AF64" s="105"/>
+      <c r="AG64" s="105"/>
+      <c r="AH64" s="105"/>
+      <c r="AI64" s="105"/>
+      <c r="AJ64" s="105"/>
+      <c r="AK64" s="105"/>
+      <c r="AL64" s="105"/>
+      <c r="AM64" s="105"/>
+      <c r="AN64" s="105"/>
+      <c r="AO64" s="105"/>
+      <c r="AP64" s="105"/>
+      <c r="AQ64" s="105"/>
+      <c r="AR64" s="105"/>
+      <c r="AS64" s="105"/>
+      <c r="AT64" s="105"/>
+      <c r="AU64" s="105"/>
+      <c r="AV64" s="105"/>
+      <c r="AW64" s="105"/>
+      <c r="AX64" s="105"/>
+      <c r="AY64" s="105"/>
+      <c r="AZ64" s="105"/>
+      <c r="BA64" s="105"/>
+      <c r="BB64" s="105"/>
+      <c r="BC64" s="105"/>
+      <c r="BD64" s="105"/>
+      <c r="BE64" s="105"/>
+      <c r="BF64" s="105"/>
+      <c r="BG64" s="105"/>
+      <c r="BH64" s="105"/>
+      <c r="BI64" s="105"/>
+      <c r="BJ64" s="105"/>
+      <c r="BK64" s="105"/>
+      <c r="BL64" s="105"/>
+      <c r="BM64" s="105"/>
+      <c r="BN64" s="105"/>
+    </row>
+    <row r="65" spans="1:66" s="55" customFormat="1" ht="18" x14ac:dyDescent="0.15">
+      <c r="A65" s="53" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>12</v>
       </c>
-      <c r="B62" s="54" t="s">
-        <v>155</v>
-      </c>
-      <c r="D62" s="56"/>
-      <c r="E62" s="161"/>
-      <c r="F62" s="161" t="str">
+      <c r="B65" s="54" t="s">
+        <v>154</v>
+      </c>
+      <c r="D65" s="56"/>
+      <c r="E65" s="161"/>
+      <c r="F65" s="161" t="str">
         <f t="shared" si="28"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="G62" s="57"/>
-      <c r="H62" s="58"/>
-      <c r="I62" s="59" t="str">
+      <c r="G65" s="57"/>
+      <c r="H65" s="58"/>
+      <c r="I65" s="59" t="str">
         <f t="shared" si="29"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="J62" s="95"/>
-      <c r="K62" s="106"/>
-      <c r="L62" s="106"/>
-      <c r="M62" s="106"/>
-      <c r="N62" s="106"/>
-      <c r="O62" s="106"/>
-      <c r="P62" s="106"/>
-      <c r="Q62" s="106"/>
-      <c r="R62" s="106"/>
-      <c r="S62" s="106"/>
-      <c r="T62" s="106"/>
-      <c r="U62" s="106"/>
-      <c r="V62" s="106"/>
-      <c r="W62" s="106"/>
-      <c r="X62" s="106"/>
-      <c r="Y62" s="106"/>
-      <c r="Z62" s="106"/>
-      <c r="AA62" s="106"/>
-      <c r="AB62" s="106"/>
-      <c r="AC62" s="106"/>
-      <c r="AD62" s="106"/>
-      <c r="AE62" s="106"/>
-      <c r="AF62" s="106"/>
-      <c r="AG62" s="106"/>
-      <c r="AH62" s="106"/>
-      <c r="AI62" s="106"/>
-      <c r="AJ62" s="106"/>
-      <c r="AK62" s="106"/>
-      <c r="AL62" s="106"/>
-      <c r="AM62" s="106"/>
-      <c r="AN62" s="106"/>
-      <c r="AO62" s="106"/>
-      <c r="AP62" s="106"/>
-      <c r="AQ62" s="106"/>
-      <c r="AR62" s="106"/>
-      <c r="AS62" s="106"/>
-      <c r="AT62" s="106"/>
-      <c r="AU62" s="106"/>
-      <c r="AV62" s="106"/>
-      <c r="AW62" s="106"/>
-      <c r="AX62" s="106"/>
-      <c r="AY62" s="106"/>
-      <c r="AZ62" s="106"/>
-      <c r="BA62" s="106"/>
-      <c r="BB62" s="106"/>
-      <c r="BC62" s="106"/>
-      <c r="BD62" s="106"/>
-      <c r="BE62" s="106"/>
-      <c r="BF62" s="106"/>
-      <c r="BG62" s="106"/>
-      <c r="BH62" s="106"/>
-      <c r="BI62" s="106"/>
-      <c r="BJ62" s="106"/>
-      <c r="BK62" s="106"/>
-      <c r="BL62" s="106"/>
-      <c r="BM62" s="106"/>
-      <c r="BN62" s="106"/>
-    </row>
-    <row r="63" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A63" s="60" t="str">
+      <c r="J65" s="95"/>
+      <c r="K65" s="106"/>
+      <c r="L65" s="106"/>
+      <c r="M65" s="106"/>
+      <c r="N65" s="106"/>
+      <c r="O65" s="106"/>
+      <c r="P65" s="106"/>
+      <c r="Q65" s="106"/>
+      <c r="R65" s="106"/>
+      <c r="S65" s="106"/>
+      <c r="T65" s="106"/>
+      <c r="U65" s="106"/>
+      <c r="V65" s="106"/>
+      <c r="W65" s="106"/>
+      <c r="X65" s="106"/>
+      <c r="Y65" s="106"/>
+      <c r="Z65" s="106"/>
+      <c r="AA65" s="106"/>
+      <c r="AB65" s="106"/>
+      <c r="AC65" s="106"/>
+      <c r="AD65" s="106"/>
+      <c r="AE65" s="106"/>
+      <c r="AF65" s="106"/>
+      <c r="AG65" s="106"/>
+      <c r="AH65" s="106"/>
+      <c r="AI65" s="106"/>
+      <c r="AJ65" s="106"/>
+      <c r="AK65" s="106"/>
+      <c r="AL65" s="106"/>
+      <c r="AM65" s="106"/>
+      <c r="AN65" s="106"/>
+      <c r="AO65" s="106"/>
+      <c r="AP65" s="106"/>
+      <c r="AQ65" s="106"/>
+      <c r="AR65" s="106"/>
+      <c r="AS65" s="106"/>
+      <c r="AT65" s="106"/>
+      <c r="AU65" s="106"/>
+      <c r="AV65" s="106"/>
+      <c r="AW65" s="106"/>
+      <c r="AX65" s="106"/>
+      <c r="AY65" s="106"/>
+      <c r="AZ65" s="106"/>
+      <c r="BA65" s="106"/>
+      <c r="BB65" s="106"/>
+      <c r="BC65" s="106"/>
+      <c r="BD65" s="106"/>
+      <c r="BE65" s="106"/>
+      <c r="BF65" s="106"/>
+      <c r="BG65" s="106"/>
+      <c r="BH65" s="106"/>
+      <c r="BI65" s="106"/>
+      <c r="BJ65" s="106"/>
+      <c r="BK65" s="106"/>
+      <c r="BL65" s="106"/>
+      <c r="BM65" s="106"/>
+      <c r="BN65" s="106"/>
+    </row>
+    <row r="66" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.15">
+      <c r="A66" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>12.1</v>
       </c>
-      <c r="B63" s="81"/>
-      <c r="C63" s="81"/>
-      <c r="D63" s="79"/>
-      <c r="E63" s="160"/>
-      <c r="F63" s="163" t="str">
+      <c r="B66" s="81"/>
+      <c r="C66" s="81"/>
+      <c r="D66" s="79"/>
+      <c r="E66" s="160"/>
+      <c r="F66" s="163" t="str">
         <f t="shared" si="28"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="G63" s="62"/>
-      <c r="H63" s="63"/>
-      <c r="I63" s="80" t="str">
+      <c r="G66" s="62"/>
+      <c r="H66" s="63"/>
+      <c r="I66" s="80" t="str">
         <f t="shared" si="29"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="J63" s="98"/>
-      <c r="K63" s="105"/>
-      <c r="L63" s="105"/>
-      <c r="M63" s="105"/>
-      <c r="N63" s="105"/>
-      <c r="O63" s="105"/>
-      <c r="P63" s="105"/>
-      <c r="Q63" s="105"/>
-      <c r="R63" s="105"/>
-      <c r="S63" s="105"/>
-      <c r="T63" s="105"/>
-      <c r="U63" s="105"/>
-      <c r="V63" s="105"/>
-      <c r="W63" s="105"/>
-      <c r="X63" s="105"/>
-      <c r="Y63" s="105"/>
-      <c r="Z63" s="105"/>
-      <c r="AA63" s="105"/>
-      <c r="AB63" s="105"/>
-      <c r="AC63" s="105"/>
-      <c r="AD63" s="105"/>
-      <c r="AE63" s="105"/>
-      <c r="AF63" s="105"/>
-      <c r="AG63" s="105"/>
-      <c r="AH63" s="105"/>
-      <c r="AI63" s="105"/>
-      <c r="AJ63" s="105"/>
-      <c r="AK63" s="105"/>
-      <c r="AL63" s="105"/>
-      <c r="AM63" s="105"/>
-      <c r="AN63" s="105"/>
-      <c r="AO63" s="105"/>
-      <c r="AP63" s="105"/>
-      <c r="AQ63" s="105"/>
-      <c r="AR63" s="105"/>
-      <c r="AS63" s="105"/>
-      <c r="AT63" s="105"/>
-      <c r="AU63" s="105"/>
-      <c r="AV63" s="105"/>
-      <c r="AW63" s="105"/>
-      <c r="AX63" s="105"/>
-      <c r="AY63" s="105"/>
-      <c r="AZ63" s="105"/>
-      <c r="BA63" s="105"/>
-      <c r="BB63" s="105"/>
-      <c r="BC63" s="105"/>
-      <c r="BD63" s="105"/>
-      <c r="BE63" s="105"/>
-      <c r="BF63" s="105"/>
-      <c r="BG63" s="105"/>
-      <c r="BH63" s="105"/>
-      <c r="BI63" s="105"/>
-      <c r="BJ63" s="105"/>
-      <c r="BK63" s="105"/>
-      <c r="BL63" s="105"/>
-      <c r="BM63" s="105"/>
-      <c r="BN63" s="105"/>
-    </row>
-    <row r="64" spans="1:66" s="55" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A64" s="53" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
-        <v>13</v>
-      </c>
-      <c r="B64" s="54" t="s">
-        <v>156</v>
-      </c>
-      <c r="D64" s="56"/>
-      <c r="E64" s="161"/>
-      <c r="F64" s="161" t="str">
-        <f t="shared" ref="F64:F65" si="36">IF(ISBLANK(E64)," - ",IF(G64=0,E64,E64+G64-1))</f>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="G64" s="57"/>
-      <c r="H64" s="58"/>
-      <c r="I64" s="59" t="str">
-        <f t="shared" ref="I64:I65" si="37">IF(OR(F64=0,E64=0)," - ",NETWORKDAYS(E64,F64))</f>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J64" s="95"/>
-      <c r="K64" s="106"/>
-      <c r="L64" s="106"/>
-      <c r="M64" s="106"/>
-      <c r="N64" s="106"/>
-      <c r="O64" s="106"/>
-      <c r="P64" s="106"/>
-      <c r="Q64" s="106"/>
-      <c r="R64" s="106"/>
-      <c r="S64" s="106"/>
-      <c r="T64" s="106"/>
-      <c r="U64" s="106"/>
-      <c r="V64" s="106"/>
-      <c r="W64" s="106"/>
-      <c r="X64" s="106"/>
-      <c r="Y64" s="106"/>
-      <c r="Z64" s="106"/>
-      <c r="AA64" s="106"/>
-      <c r="AB64" s="106"/>
-      <c r="AC64" s="106"/>
-      <c r="AD64" s="106"/>
-      <c r="AE64" s="106"/>
-      <c r="AF64" s="106"/>
-      <c r="AG64" s="106"/>
-      <c r="AH64" s="106"/>
-      <c r="AI64" s="106"/>
-      <c r="AJ64" s="106"/>
-      <c r="AK64" s="106"/>
-      <c r="AL64" s="106"/>
-      <c r="AM64" s="106"/>
-      <c r="AN64" s="106"/>
-      <c r="AO64" s="106"/>
-      <c r="AP64" s="106"/>
-      <c r="AQ64" s="106"/>
-      <c r="AR64" s="106"/>
-      <c r="AS64" s="106"/>
-      <c r="AT64" s="106"/>
-      <c r="AU64" s="106"/>
-      <c r="AV64" s="106"/>
-      <c r="AW64" s="106"/>
-      <c r="AX64" s="106"/>
-      <c r="AY64" s="106"/>
-      <c r="AZ64" s="106"/>
-      <c r="BA64" s="106"/>
-      <c r="BB64" s="106"/>
-      <c r="BC64" s="106"/>
-      <c r="BD64" s="106"/>
-      <c r="BE64" s="106"/>
-      <c r="BF64" s="106"/>
-      <c r="BG64" s="106"/>
-      <c r="BH64" s="106"/>
-      <c r="BI64" s="106"/>
-      <c r="BJ64" s="106"/>
-      <c r="BK64" s="106"/>
-      <c r="BL64" s="106"/>
-      <c r="BM64" s="106"/>
-      <c r="BN64" s="106"/>
-    </row>
-    <row r="65" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A65" s="60" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>13.1</v>
-      </c>
-      <c r="B65" s="81"/>
-      <c r="C65" s="81"/>
-      <c r="D65" s="79"/>
-      <c r="E65" s="160"/>
-      <c r="F65" s="163" t="str">
-        <f t="shared" si="36"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="G65" s="62"/>
-      <c r="H65" s="63"/>
-      <c r="I65" s="80" t="str">
-        <f t="shared" si="37"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J65" s="98"/>
-      <c r="K65" s="105"/>
-      <c r="L65" s="105"/>
-      <c r="M65" s="105"/>
-      <c r="N65" s="105"/>
-      <c r="O65" s="105"/>
-      <c r="P65" s="105"/>
-      <c r="Q65" s="105"/>
-      <c r="R65" s="105"/>
-      <c r="S65" s="105"/>
-      <c r="T65" s="105"/>
-      <c r="U65" s="105"/>
-      <c r="V65" s="105"/>
-      <c r="W65" s="105"/>
-      <c r="X65" s="105"/>
-      <c r="Y65" s="105"/>
-      <c r="Z65" s="105"/>
-      <c r="AA65" s="105"/>
-      <c r="AB65" s="105"/>
-      <c r="AC65" s="105"/>
-      <c r="AD65" s="105"/>
-      <c r="AE65" s="105"/>
-      <c r="AF65" s="105"/>
-      <c r="AG65" s="105"/>
-      <c r="AH65" s="105"/>
-      <c r="AI65" s="105"/>
-      <c r="AJ65" s="105"/>
-      <c r="AK65" s="105"/>
-      <c r="AL65" s="105"/>
-      <c r="AM65" s="105"/>
-      <c r="AN65" s="105"/>
-      <c r="AO65" s="105"/>
-      <c r="AP65" s="105"/>
-      <c r="AQ65" s="105"/>
-      <c r="AR65" s="105"/>
-      <c r="AS65" s="105"/>
-      <c r="AT65" s="105"/>
-      <c r="AU65" s="105"/>
-      <c r="AV65" s="105"/>
-      <c r="AW65" s="105"/>
-      <c r="AX65" s="105"/>
-      <c r="AY65" s="105"/>
-      <c r="AZ65" s="105"/>
-      <c r="BA65" s="105"/>
-      <c r="BB65" s="105"/>
-      <c r="BC65" s="105"/>
-      <c r="BD65" s="105"/>
-      <c r="BE65" s="105"/>
-      <c r="BF65" s="105"/>
-      <c r="BG65" s="105"/>
-      <c r="BH65" s="105"/>
-      <c r="BI65" s="105"/>
-      <c r="BJ65" s="105"/>
-      <c r="BK65" s="105"/>
-      <c r="BL65" s="105"/>
-      <c r="BM65" s="105"/>
-      <c r="BN65" s="105"/>
-    </row>
-    <row r="66" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A66" s="60"/>
-      <c r="B66" s="65"/>
-      <c r="C66" s="65"/>
-      <c r="D66" s="66"/>
-      <c r="E66" s="101"/>
-      <c r="F66" s="101"/>
-      <c r="G66" s="67"/>
-      <c r="H66" s="68"/>
-      <c r="I66" s="69" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J66" s="96"/>
+      <c r="J66" s="98"/>
       <c r="K66" s="105"/>
       <c r="L66" s="105"/>
       <c r="M66" s="105"/>
@@ -9857,89 +10044,104 @@
       <c r="BM66" s="105"/>
       <c r="BN66" s="105"/>
     </row>
-    <row r="67" spans="1:66" s="75" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A67" s="71" t="s">
-        <v>1</v>
-      </c>
-      <c r="B67" s="72"/>
-      <c r="C67" s="73"/>
-      <c r="D67" s="73"/>
-      <c r="E67" s="102"/>
-      <c r="F67" s="102"/>
-      <c r="G67" s="74"/>
-      <c r="H67" s="74"/>
-      <c r="I67" s="74"/>
-      <c r="J67" s="97"/>
-      <c r="K67" s="105"/>
-      <c r="L67" s="105"/>
-      <c r="M67" s="105"/>
-      <c r="N67" s="105"/>
-      <c r="O67" s="105"/>
-      <c r="P67" s="105"/>
-      <c r="Q67" s="105"/>
-      <c r="R67" s="105"/>
-      <c r="S67" s="105"/>
-      <c r="T67" s="105"/>
-      <c r="U67" s="105"/>
-      <c r="V67" s="105"/>
-      <c r="W67" s="105"/>
-      <c r="X67" s="105"/>
-      <c r="Y67" s="105"/>
-      <c r="Z67" s="105"/>
-      <c r="AA67" s="105"/>
-      <c r="AB67" s="105"/>
-      <c r="AC67" s="105"/>
-      <c r="AD67" s="105"/>
-      <c r="AE67" s="105"/>
-      <c r="AF67" s="105"/>
-      <c r="AG67" s="105"/>
-      <c r="AH67" s="105"/>
-      <c r="AI67" s="105"/>
-      <c r="AJ67" s="105"/>
-      <c r="AK67" s="105"/>
-      <c r="AL67" s="105"/>
-      <c r="AM67" s="105"/>
-      <c r="AN67" s="105"/>
-      <c r="AO67" s="105"/>
-      <c r="AP67" s="105"/>
-      <c r="AQ67" s="105"/>
-      <c r="AR67" s="105"/>
-      <c r="AS67" s="105"/>
-      <c r="AT67" s="105"/>
-      <c r="AU67" s="105"/>
-      <c r="AV67" s="105"/>
-      <c r="AW67" s="105"/>
-      <c r="AX67" s="105"/>
-      <c r="AY67" s="105"/>
-      <c r="AZ67" s="105"/>
-      <c r="BA67" s="105"/>
-      <c r="BB67" s="105"/>
-      <c r="BC67" s="105"/>
-      <c r="BD67" s="105"/>
-      <c r="BE67" s="105"/>
-      <c r="BF67" s="105"/>
-      <c r="BG67" s="105"/>
-      <c r="BH67" s="105"/>
-      <c r="BI67" s="105"/>
-      <c r="BJ67" s="105"/>
-      <c r="BK67" s="105"/>
-      <c r="BL67" s="105"/>
-      <c r="BM67" s="105"/>
-      <c r="BN67" s="105"/>
+    <row r="67" spans="1:66" s="55" customFormat="1" ht="18" x14ac:dyDescent="0.15">
+      <c r="A67" s="53" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+        <v>13</v>
+      </c>
+      <c r="B67" s="54" t="s">
+        <v>155</v>
+      </c>
+      <c r="D67" s="56"/>
+      <c r="E67" s="161"/>
+      <c r="F67" s="161" t="str">
+        <f t="shared" si="28"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="G67" s="57"/>
+      <c r="H67" s="58"/>
+      <c r="I67" s="59" t="str">
+        <f t="shared" si="29"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J67" s="95"/>
+      <c r="K67" s="106"/>
+      <c r="L67" s="106"/>
+      <c r="M67" s="106"/>
+      <c r="N67" s="106"/>
+      <c r="O67" s="106"/>
+      <c r="P67" s="106"/>
+      <c r="Q67" s="106"/>
+      <c r="R67" s="106"/>
+      <c r="S67" s="106"/>
+      <c r="T67" s="106"/>
+      <c r="U67" s="106"/>
+      <c r="V67" s="106"/>
+      <c r="W67" s="106"/>
+      <c r="X67" s="106"/>
+      <c r="Y67" s="106"/>
+      <c r="Z67" s="106"/>
+      <c r="AA67" s="106"/>
+      <c r="AB67" s="106"/>
+      <c r="AC67" s="106"/>
+      <c r="AD67" s="106"/>
+      <c r="AE67" s="106"/>
+      <c r="AF67" s="106"/>
+      <c r="AG67" s="106"/>
+      <c r="AH67" s="106"/>
+      <c r="AI67" s="106"/>
+      <c r="AJ67" s="106"/>
+      <c r="AK67" s="106"/>
+      <c r="AL67" s="106"/>
+      <c r="AM67" s="106"/>
+      <c r="AN67" s="106"/>
+      <c r="AO67" s="106"/>
+      <c r="AP67" s="106"/>
+      <c r="AQ67" s="106"/>
+      <c r="AR67" s="106"/>
+      <c r="AS67" s="106"/>
+      <c r="AT67" s="106"/>
+      <c r="AU67" s="106"/>
+      <c r="AV67" s="106"/>
+      <c r="AW67" s="106"/>
+      <c r="AX67" s="106"/>
+      <c r="AY67" s="106"/>
+      <c r="AZ67" s="106"/>
+      <c r="BA67" s="106"/>
+      <c r="BB67" s="106"/>
+      <c r="BC67" s="106"/>
+      <c r="BD67" s="106"/>
+      <c r="BE67" s="106"/>
+      <c r="BF67" s="106"/>
+      <c r="BG67" s="106"/>
+      <c r="BH67" s="106"/>
+      <c r="BI67" s="106"/>
+      <c r="BJ67" s="106"/>
+      <c r="BK67" s="106"/>
+      <c r="BL67" s="106"/>
+      <c r="BM67" s="106"/>
+      <c r="BN67" s="106"/>
     </row>
     <row r="68" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A68" s="76" t="s">
-        <v>37</v>
-      </c>
-      <c r="B68" s="77"/>
-      <c r="C68" s="77"/>
-      <c r="D68" s="77"/>
-      <c r="E68" s="103"/>
-      <c r="F68" s="103"/>
-      <c r="G68" s="77"/>
-      <c r="H68" s="77"/>
-      <c r="I68" s="77"/>
-      <c r="J68" s="97"/>
+      <c r="A68" s="60" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>13.1</v>
+      </c>
+      <c r="B68" s="81"/>
+      <c r="C68" s="81"/>
+      <c r="D68" s="79"/>
+      <c r="E68" s="160"/>
+      <c r="F68" s="163" t="str">
+        <f t="shared" si="28"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="G68" s="62"/>
+      <c r="H68" s="63"/>
+      <c r="I68" s="80" t="str">
+        <f t="shared" si="29"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J68" s="98"/>
       <c r="K68" s="105"/>
       <c r="L68" s="105"/>
       <c r="M68" s="105"/>
@@ -9997,104 +10199,101 @@
       <c r="BM68" s="105"/>
       <c r="BN68" s="105"/>
     </row>
-    <row r="69" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A69" s="124" t="str">
+    <row r="69" spans="1:66" s="55" customFormat="1" ht="18" x14ac:dyDescent="0.15">
+      <c r="A69" s="53" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
-        <v>1</v>
-      </c>
-      <c r="B69" s="125" t="s">
-        <v>76</v>
-      </c>
-      <c r="C69" s="78"/>
-      <c r="D69" s="79"/>
-      <c r="E69" s="99"/>
-      <c r="F69" s="100" t="str">
-        <f t="shared" ref="F69:F72" si="38">IF(ISBLANK(E69)," - ",IF(G69=0,E69,E69+G69-1))</f>
+        <v>14</v>
+      </c>
+      <c r="B69" s="54" t="s">
+        <v>156</v>
+      </c>
+      <c r="D69" s="56"/>
+      <c r="E69" s="161"/>
+      <c r="F69" s="161" t="str">
+        <f t="shared" ref="F69:F70" si="38">IF(ISBLANK(E69)," - ",IF(G69=0,E69,E69+G69-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="G69" s="62"/>
-      <c r="H69" s="63"/>
-      <c r="I69" s="80" t="str">
-        <f>IF(OR(F69=0,E69=0)," - ",NETWORKDAYS(E69,F69))</f>
+      <c r="G69" s="57"/>
+      <c r="H69" s="58"/>
+      <c r="I69" s="59" t="str">
+        <f t="shared" ref="I69:I70" si="39">IF(OR(F69=0,E69=0)," - ",NETWORKDAYS(E69,F69))</f>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="J69" s="98"/>
-      <c r="K69" s="105"/>
-      <c r="L69" s="105"/>
-      <c r="M69" s="105"/>
-      <c r="N69" s="105"/>
-      <c r="O69" s="105"/>
-      <c r="P69" s="105"/>
-      <c r="Q69" s="105"/>
-      <c r="R69" s="105"/>
-      <c r="S69" s="105"/>
-      <c r="T69" s="105"/>
-      <c r="U69" s="105"/>
-      <c r="V69" s="105"/>
-      <c r="W69" s="105"/>
-      <c r="X69" s="105"/>
-      <c r="Y69" s="105"/>
-      <c r="Z69" s="105"/>
-      <c r="AA69" s="105"/>
-      <c r="AB69" s="105"/>
-      <c r="AC69" s="105"/>
-      <c r="AD69" s="105"/>
-      <c r="AE69" s="105"/>
-      <c r="AF69" s="105"/>
-      <c r="AG69" s="105"/>
-      <c r="AH69" s="105"/>
-      <c r="AI69" s="105"/>
-      <c r="AJ69" s="105"/>
-      <c r="AK69" s="105"/>
-      <c r="AL69" s="105"/>
-      <c r="AM69" s="105"/>
-      <c r="AN69" s="105"/>
-      <c r="AO69" s="105"/>
-      <c r="AP69" s="105"/>
-      <c r="AQ69" s="105"/>
-      <c r="AR69" s="105"/>
-      <c r="AS69" s="105"/>
-      <c r="AT69" s="105"/>
-      <c r="AU69" s="105"/>
-      <c r="AV69" s="105"/>
-      <c r="AW69" s="105"/>
-      <c r="AX69" s="105"/>
-      <c r="AY69" s="105"/>
-      <c r="AZ69" s="105"/>
-      <c r="BA69" s="105"/>
-      <c r="BB69" s="105"/>
-      <c r="BC69" s="105"/>
-      <c r="BD69" s="105"/>
-      <c r="BE69" s="105"/>
-      <c r="BF69" s="105"/>
-      <c r="BG69" s="105"/>
-      <c r="BH69" s="105"/>
-      <c r="BI69" s="105"/>
-      <c r="BJ69" s="105"/>
-      <c r="BK69" s="105"/>
-      <c r="BL69" s="105"/>
-      <c r="BM69" s="105"/>
-      <c r="BN69" s="105"/>
+      <c r="J69" s="95"/>
+      <c r="K69" s="106"/>
+      <c r="L69" s="106"/>
+      <c r="M69" s="106"/>
+      <c r="N69" s="106"/>
+      <c r="O69" s="106"/>
+      <c r="P69" s="106"/>
+      <c r="Q69" s="106"/>
+      <c r="R69" s="106"/>
+      <c r="S69" s="106"/>
+      <c r="T69" s="106"/>
+      <c r="U69" s="106"/>
+      <c r="V69" s="106"/>
+      <c r="W69" s="106"/>
+      <c r="X69" s="106"/>
+      <c r="Y69" s="106"/>
+      <c r="Z69" s="106"/>
+      <c r="AA69" s="106"/>
+      <c r="AB69" s="106"/>
+      <c r="AC69" s="106"/>
+      <c r="AD69" s="106"/>
+      <c r="AE69" s="106"/>
+      <c r="AF69" s="106"/>
+      <c r="AG69" s="106"/>
+      <c r="AH69" s="106"/>
+      <c r="AI69" s="106"/>
+      <c r="AJ69" s="106"/>
+      <c r="AK69" s="106"/>
+      <c r="AL69" s="106"/>
+      <c r="AM69" s="106"/>
+      <c r="AN69" s="106"/>
+      <c r="AO69" s="106"/>
+      <c r="AP69" s="106"/>
+      <c r="AQ69" s="106"/>
+      <c r="AR69" s="106"/>
+      <c r="AS69" s="106"/>
+      <c r="AT69" s="106"/>
+      <c r="AU69" s="106"/>
+      <c r="AV69" s="106"/>
+      <c r="AW69" s="106"/>
+      <c r="AX69" s="106"/>
+      <c r="AY69" s="106"/>
+      <c r="AZ69" s="106"/>
+      <c r="BA69" s="106"/>
+      <c r="BB69" s="106"/>
+      <c r="BC69" s="106"/>
+      <c r="BD69" s="106"/>
+      <c r="BE69" s="106"/>
+      <c r="BF69" s="106"/>
+      <c r="BG69" s="106"/>
+      <c r="BH69" s="106"/>
+      <c r="BI69" s="106"/>
+      <c r="BJ69" s="106"/>
+      <c r="BK69" s="106"/>
+      <c r="BL69" s="106"/>
+      <c r="BM69" s="106"/>
+      <c r="BN69" s="106"/>
     </row>
     <row r="70" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.15">
       <c r="A70" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>1.1</v>
-      </c>
-      <c r="B70" s="81" t="s">
-        <v>62</v>
-      </c>
+        <v>14.1</v>
+      </c>
+      <c r="B70" s="81"/>
       <c r="C70" s="81"/>
       <c r="D70" s="79"/>
-      <c r="E70" s="99"/>
-      <c r="F70" s="100" t="str">
+      <c r="E70" s="160"/>
+      <c r="F70" s="163" t="str">
         <f t="shared" si="38"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G70" s="62"/>
       <c r="H70" s="63"/>
       <c r="I70" s="80" t="str">
-        <f t="shared" ref="I70:I72" si="39">IF(OR(F70=0,E70=0)," - ",NETWORKDAYS(E70,F70))</f>
+        <f t="shared" si="39"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J70" s="98"/>
@@ -10156,27 +10355,19 @@
       <c r="BN70" s="105"/>
     </row>
     <row r="71" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A71" s="60" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
-        <v>1.1.1</v>
-      </c>
-      <c r="B71" s="82" t="s">
-        <v>63</v>
-      </c>
-      <c r="C71" s="81"/>
-      <c r="D71" s="79"/>
-      <c r="E71" s="99"/>
-      <c r="F71" s="100" t="str">
-        <f t="shared" si="38"/>
+      <c r="A71" s="60"/>
+      <c r="B71" s="65"/>
+      <c r="C71" s="65"/>
+      <c r="D71" s="66"/>
+      <c r="E71" s="101"/>
+      <c r="F71" s="101"/>
+      <c r="G71" s="67"/>
+      <c r="H71" s="68"/>
+      <c r="I71" s="69" t="str">
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="G71" s="62"/>
-      <c r="H71" s="63"/>
-      <c r="I71" s="80" t="str">
-        <f t="shared" si="39"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J71" s="98"/>
+      <c r="J71" s="96"/>
       <c r="K71" s="105"/>
       <c r="L71" s="105"/>
       <c r="M71" s="105"/>
@@ -10234,28 +10425,19 @@
       <c r="BM71" s="105"/>
       <c r="BN71" s="105"/>
     </row>
-    <row r="72" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A72" s="60" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",4))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",3))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",4))-FIND("`",SUBSTITUTE(prevWBS,".","`",3))-1)))+1)))</f>
-        <v>1.1.1.1</v>
-      </c>
-      <c r="B72" s="82" t="s">
-        <v>64</v>
-      </c>
-      <c r="C72" s="81"/>
-      <c r="D72" s="79"/>
-      <c r="E72" s="99"/>
-      <c r="F72" s="100" t="str">
-        <f t="shared" si="38"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="G72" s="62"/>
-      <c r="H72" s="63"/>
-      <c r="I72" s="80" t="str">
-        <f t="shared" si="39"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J72" s="98"/>
+    <row r="72" spans="1:66" s="75" customFormat="1" ht="18" x14ac:dyDescent="0.15">
+      <c r="A72" s="71" t="s">
+        <v>1</v>
+      </c>
+      <c r="B72" s="72"/>
+      <c r="C72" s="73"/>
+      <c r="D72" s="73"/>
+      <c r="E72" s="102"/>
+      <c r="F72" s="102"/>
+      <c r="G72" s="74"/>
+      <c r="H72" s="74"/>
+      <c r="I72" s="74"/>
+      <c r="J72" s="97"/>
       <c r="K72" s="105"/>
       <c r="L72" s="105"/>
       <c r="M72" s="105"/>
@@ -10313,86 +10495,463 @@
       <c r="BM72" s="105"/>
       <c r="BN72" s="105"/>
     </row>
-    <row r="73" spans="1:66" s="33" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A73" s="30"/>
-      <c r="B73" s="31"/>
-      <c r="C73" s="31"/>
-      <c r="D73" s="32"/>
-      <c r="E73" s="31"/>
-      <c r="F73" s="31"/>
-      <c r="G73" s="31"/>
-      <c r="H73" s="31"/>
-      <c r="I73" s="31"/>
-      <c r="J73" s="31"/>
-      <c r="K73" s="31"/>
-      <c r="L73" s="31"/>
-      <c r="M73" s="31"/>
-      <c r="N73" s="31"/>
-      <c r="O73" s="31"/>
-      <c r="P73" s="31"/>
-      <c r="Q73" s="31"/>
-      <c r="R73" s="31"/>
-      <c r="S73" s="31"/>
-      <c r="T73" s="31"/>
-      <c r="U73" s="31"/>
-      <c r="V73" s="31"/>
-      <c r="W73" s="31"/>
-      <c r="X73" s="31"/>
-      <c r="Y73" s="31"/>
-      <c r="Z73" s="31"/>
-      <c r="AA73" s="31"/>
-      <c r="AB73" s="31"/>
-      <c r="AC73" s="31"/>
-      <c r="AD73" s="31"/>
-      <c r="AE73" s="31"/>
-      <c r="AF73" s="31"/>
-      <c r="AG73" s="31"/>
-      <c r="AH73" s="31"/>
-      <c r="AI73" s="31"/>
-      <c r="AJ73" s="31"/>
-      <c r="AK73" s="31"/>
-      <c r="AL73" s="31"/>
-      <c r="AM73" s="31"/>
-      <c r="AN73" s="31"/>
-      <c r="AO73" s="31"/>
-      <c r="AP73" s="31"/>
-      <c r="AQ73" s="31"/>
-      <c r="AR73" s="31"/>
-      <c r="AS73" s="31"/>
-      <c r="AT73" s="31"/>
-      <c r="AU73" s="31"/>
-      <c r="AV73" s="31"/>
-      <c r="AW73" s="31"/>
-      <c r="AX73" s="31"/>
-      <c r="AY73" s="31"/>
-      <c r="AZ73" s="31"/>
-      <c r="BA73" s="31"/>
-      <c r="BB73" s="31"/>
-      <c r="BC73" s="31"/>
-      <c r="BD73" s="31"/>
-      <c r="BE73" s="31"/>
-      <c r="BF73" s="31"/>
-      <c r="BG73" s="31"/>
-      <c r="BH73" s="31"/>
-      <c r="BI73" s="31"/>
-      <c r="BJ73" s="31"/>
-      <c r="BK73" s="31"/>
-      <c r="BL73" s="31"/>
-      <c r="BM73" s="31"/>
-      <c r="BN73" s="31"/>
+    <row r="73" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.15">
+      <c r="A73" s="76" t="s">
+        <v>37</v>
+      </c>
+      <c r="B73" s="77"/>
+      <c r="C73" s="77"/>
+      <c r="D73" s="77"/>
+      <c r="E73" s="103"/>
+      <c r="F73" s="103"/>
+      <c r="G73" s="77"/>
+      <c r="H73" s="77"/>
+      <c r="I73" s="77"/>
+      <c r="J73" s="97"/>
+      <c r="K73" s="105"/>
+      <c r="L73" s="105"/>
+      <c r="M73" s="105"/>
+      <c r="N73" s="105"/>
+      <c r="O73" s="105"/>
+      <c r="P73" s="105"/>
+      <c r="Q73" s="105"/>
+      <c r="R73" s="105"/>
+      <c r="S73" s="105"/>
+      <c r="T73" s="105"/>
+      <c r="U73" s="105"/>
+      <c r="V73" s="105"/>
+      <c r="W73" s="105"/>
+      <c r="X73" s="105"/>
+      <c r="Y73" s="105"/>
+      <c r="Z73" s="105"/>
+      <c r="AA73" s="105"/>
+      <c r="AB73" s="105"/>
+      <c r="AC73" s="105"/>
+      <c r="AD73" s="105"/>
+      <c r="AE73" s="105"/>
+      <c r="AF73" s="105"/>
+      <c r="AG73" s="105"/>
+      <c r="AH73" s="105"/>
+      <c r="AI73" s="105"/>
+      <c r="AJ73" s="105"/>
+      <c r="AK73" s="105"/>
+      <c r="AL73" s="105"/>
+      <c r="AM73" s="105"/>
+      <c r="AN73" s="105"/>
+      <c r="AO73" s="105"/>
+      <c r="AP73" s="105"/>
+      <c r="AQ73" s="105"/>
+      <c r="AR73" s="105"/>
+      <c r="AS73" s="105"/>
+      <c r="AT73" s="105"/>
+      <c r="AU73" s="105"/>
+      <c r="AV73" s="105"/>
+      <c r="AW73" s="105"/>
+      <c r="AX73" s="105"/>
+      <c r="AY73" s="105"/>
+      <c r="AZ73" s="105"/>
+      <c r="BA73" s="105"/>
+      <c r="BB73" s="105"/>
+      <c r="BC73" s="105"/>
+      <c r="BD73" s="105"/>
+      <c r="BE73" s="105"/>
+      <c r="BF73" s="105"/>
+      <c r="BG73" s="105"/>
+      <c r="BH73" s="105"/>
+      <c r="BI73" s="105"/>
+      <c r="BJ73" s="105"/>
+      <c r="BK73" s="105"/>
+      <c r="BL73" s="105"/>
+      <c r="BM73" s="105"/>
+      <c r="BN73" s="105"/>
+    </row>
+    <row r="74" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.15">
+      <c r="A74" s="124" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+        <v>1</v>
+      </c>
+      <c r="B74" s="125" t="s">
+        <v>76</v>
+      </c>
+      <c r="C74" s="78"/>
+      <c r="D74" s="79"/>
+      <c r="E74" s="99"/>
+      <c r="F74" s="100" t="str">
+        <f t="shared" ref="F74:F77" si="40">IF(ISBLANK(E74)," - ",IF(G74=0,E74,E74+G74-1))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="G74" s="62"/>
+      <c r="H74" s="63"/>
+      <c r="I74" s="80" t="str">
+        <f>IF(OR(F74=0,E74=0)," - ",NETWORKDAYS(E74,F74))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J74" s="98"/>
+      <c r="K74" s="105"/>
+      <c r="L74" s="105"/>
+      <c r="M74" s="105"/>
+      <c r="N74" s="105"/>
+      <c r="O74" s="105"/>
+      <c r="P74" s="105"/>
+      <c r="Q74" s="105"/>
+      <c r="R74" s="105"/>
+      <c r="S74" s="105"/>
+      <c r="T74" s="105"/>
+      <c r="U74" s="105"/>
+      <c r="V74" s="105"/>
+      <c r="W74" s="105"/>
+      <c r="X74" s="105"/>
+      <c r="Y74" s="105"/>
+      <c r="Z74" s="105"/>
+      <c r="AA74" s="105"/>
+      <c r="AB74" s="105"/>
+      <c r="AC74" s="105"/>
+      <c r="AD74" s="105"/>
+      <c r="AE74" s="105"/>
+      <c r="AF74" s="105"/>
+      <c r="AG74" s="105"/>
+      <c r="AH74" s="105"/>
+      <c r="AI74" s="105"/>
+      <c r="AJ74" s="105"/>
+      <c r="AK74" s="105"/>
+      <c r="AL74" s="105"/>
+      <c r="AM74" s="105"/>
+      <c r="AN74" s="105"/>
+      <c r="AO74" s="105"/>
+      <c r="AP74" s="105"/>
+      <c r="AQ74" s="105"/>
+      <c r="AR74" s="105"/>
+      <c r="AS74" s="105"/>
+      <c r="AT74" s="105"/>
+      <c r="AU74" s="105"/>
+      <c r="AV74" s="105"/>
+      <c r="AW74" s="105"/>
+      <c r="AX74" s="105"/>
+      <c r="AY74" s="105"/>
+      <c r="AZ74" s="105"/>
+      <c r="BA74" s="105"/>
+      <c r="BB74" s="105"/>
+      <c r="BC74" s="105"/>
+      <c r="BD74" s="105"/>
+      <c r="BE74" s="105"/>
+      <c r="BF74" s="105"/>
+      <c r="BG74" s="105"/>
+      <c r="BH74" s="105"/>
+      <c r="BI74" s="105"/>
+      <c r="BJ74" s="105"/>
+      <c r="BK74" s="105"/>
+      <c r="BL74" s="105"/>
+      <c r="BM74" s="105"/>
+      <c r="BN74" s="105"/>
+    </row>
+    <row r="75" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.15">
+      <c r="A75" s="60" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>1.1</v>
+      </c>
+      <c r="B75" s="81" t="s">
+        <v>62</v>
+      </c>
+      <c r="C75" s="81"/>
+      <c r="D75" s="79"/>
+      <c r="E75" s="99"/>
+      <c r="F75" s="100" t="str">
+        <f t="shared" si="40"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="G75" s="62"/>
+      <c r="H75" s="63"/>
+      <c r="I75" s="80" t="str">
+        <f t="shared" ref="I75:I77" si="41">IF(OR(F75=0,E75=0)," - ",NETWORKDAYS(E75,F75))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J75" s="98"/>
+      <c r="K75" s="105"/>
+      <c r="L75" s="105"/>
+      <c r="M75" s="105"/>
+      <c r="N75" s="105"/>
+      <c r="O75" s="105"/>
+      <c r="P75" s="105"/>
+      <c r="Q75" s="105"/>
+      <c r="R75" s="105"/>
+      <c r="S75" s="105"/>
+      <c r="T75" s="105"/>
+      <c r="U75" s="105"/>
+      <c r="V75" s="105"/>
+      <c r="W75" s="105"/>
+      <c r="X75" s="105"/>
+      <c r="Y75" s="105"/>
+      <c r="Z75" s="105"/>
+      <c r="AA75" s="105"/>
+      <c r="AB75" s="105"/>
+      <c r="AC75" s="105"/>
+      <c r="AD75" s="105"/>
+      <c r="AE75" s="105"/>
+      <c r="AF75" s="105"/>
+      <c r="AG75" s="105"/>
+      <c r="AH75" s="105"/>
+      <c r="AI75" s="105"/>
+      <c r="AJ75" s="105"/>
+      <c r="AK75" s="105"/>
+      <c r="AL75" s="105"/>
+      <c r="AM75" s="105"/>
+      <c r="AN75" s="105"/>
+      <c r="AO75" s="105"/>
+      <c r="AP75" s="105"/>
+      <c r="AQ75" s="105"/>
+      <c r="AR75" s="105"/>
+      <c r="AS75" s="105"/>
+      <c r="AT75" s="105"/>
+      <c r="AU75" s="105"/>
+      <c r="AV75" s="105"/>
+      <c r="AW75" s="105"/>
+      <c r="AX75" s="105"/>
+      <c r="AY75" s="105"/>
+      <c r="AZ75" s="105"/>
+      <c r="BA75" s="105"/>
+      <c r="BB75" s="105"/>
+      <c r="BC75" s="105"/>
+      <c r="BD75" s="105"/>
+      <c r="BE75" s="105"/>
+      <c r="BF75" s="105"/>
+      <c r="BG75" s="105"/>
+      <c r="BH75" s="105"/>
+      <c r="BI75" s="105"/>
+      <c r="BJ75" s="105"/>
+      <c r="BK75" s="105"/>
+      <c r="BL75" s="105"/>
+      <c r="BM75" s="105"/>
+      <c r="BN75" s="105"/>
+    </row>
+    <row r="76" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.15">
+      <c r="A76" s="60" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
+        <v>1.1.1</v>
+      </c>
+      <c r="B76" s="82" t="s">
+        <v>63</v>
+      </c>
+      <c r="C76" s="81"/>
+      <c r="D76" s="79"/>
+      <c r="E76" s="99"/>
+      <c r="F76" s="100" t="str">
+        <f t="shared" si="40"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="G76" s="62"/>
+      <c r="H76" s="63"/>
+      <c r="I76" s="80" t="str">
+        <f t="shared" si="41"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J76" s="98"/>
+      <c r="K76" s="105"/>
+      <c r="L76" s="105"/>
+      <c r="M76" s="105"/>
+      <c r="N76" s="105"/>
+      <c r="O76" s="105"/>
+      <c r="P76" s="105"/>
+      <c r="Q76" s="105"/>
+      <c r="R76" s="105"/>
+      <c r="S76" s="105"/>
+      <c r="T76" s="105"/>
+      <c r="U76" s="105"/>
+      <c r="V76" s="105"/>
+      <c r="W76" s="105"/>
+      <c r="X76" s="105"/>
+      <c r="Y76" s="105"/>
+      <c r="Z76" s="105"/>
+      <c r="AA76" s="105"/>
+      <c r="AB76" s="105"/>
+      <c r="AC76" s="105"/>
+      <c r="AD76" s="105"/>
+      <c r="AE76" s="105"/>
+      <c r="AF76" s="105"/>
+      <c r="AG76" s="105"/>
+      <c r="AH76" s="105"/>
+      <c r="AI76" s="105"/>
+      <c r="AJ76" s="105"/>
+      <c r="AK76" s="105"/>
+      <c r="AL76" s="105"/>
+      <c r="AM76" s="105"/>
+      <c r="AN76" s="105"/>
+      <c r="AO76" s="105"/>
+      <c r="AP76" s="105"/>
+      <c r="AQ76" s="105"/>
+      <c r="AR76" s="105"/>
+      <c r="AS76" s="105"/>
+      <c r="AT76" s="105"/>
+      <c r="AU76" s="105"/>
+      <c r="AV76" s="105"/>
+      <c r="AW76" s="105"/>
+      <c r="AX76" s="105"/>
+      <c r="AY76" s="105"/>
+      <c r="AZ76" s="105"/>
+      <c r="BA76" s="105"/>
+      <c r="BB76" s="105"/>
+      <c r="BC76" s="105"/>
+      <c r="BD76" s="105"/>
+      <c r="BE76" s="105"/>
+      <c r="BF76" s="105"/>
+      <c r="BG76" s="105"/>
+      <c r="BH76" s="105"/>
+      <c r="BI76" s="105"/>
+      <c r="BJ76" s="105"/>
+      <c r="BK76" s="105"/>
+      <c r="BL76" s="105"/>
+      <c r="BM76" s="105"/>
+      <c r="BN76" s="105"/>
+    </row>
+    <row r="77" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.15">
+      <c r="A77" s="60" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",4))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",3))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",4))-FIND("`",SUBSTITUTE(prevWBS,".","`",3))-1)))+1)))</f>
+        <v>1.1.1.1</v>
+      </c>
+      <c r="B77" s="82" t="s">
+        <v>64</v>
+      </c>
+      <c r="C77" s="81"/>
+      <c r="D77" s="79"/>
+      <c r="E77" s="99"/>
+      <c r="F77" s="100" t="str">
+        <f t="shared" si="40"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="G77" s="62"/>
+      <c r="H77" s="63"/>
+      <c r="I77" s="80" t="str">
+        <f t="shared" si="41"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J77" s="98"/>
+      <c r="K77" s="105"/>
+      <c r="L77" s="105"/>
+      <c r="M77" s="105"/>
+      <c r="N77" s="105"/>
+      <c r="O77" s="105"/>
+      <c r="P77" s="105"/>
+      <c r="Q77" s="105"/>
+      <c r="R77" s="105"/>
+      <c r="S77" s="105"/>
+      <c r="T77" s="105"/>
+      <c r="U77" s="105"/>
+      <c r="V77" s="105"/>
+      <c r="W77" s="105"/>
+      <c r="X77" s="105"/>
+      <c r="Y77" s="105"/>
+      <c r="Z77" s="105"/>
+      <c r="AA77" s="105"/>
+      <c r="AB77" s="105"/>
+      <c r="AC77" s="105"/>
+      <c r="AD77" s="105"/>
+      <c r="AE77" s="105"/>
+      <c r="AF77" s="105"/>
+      <c r="AG77" s="105"/>
+      <c r="AH77" s="105"/>
+      <c r="AI77" s="105"/>
+      <c r="AJ77" s="105"/>
+      <c r="AK77" s="105"/>
+      <c r="AL77" s="105"/>
+      <c r="AM77" s="105"/>
+      <c r="AN77" s="105"/>
+      <c r="AO77" s="105"/>
+      <c r="AP77" s="105"/>
+      <c r="AQ77" s="105"/>
+      <c r="AR77" s="105"/>
+      <c r="AS77" s="105"/>
+      <c r="AT77" s="105"/>
+      <c r="AU77" s="105"/>
+      <c r="AV77" s="105"/>
+      <c r="AW77" s="105"/>
+      <c r="AX77" s="105"/>
+      <c r="AY77" s="105"/>
+      <c r="AZ77" s="105"/>
+      <c r="BA77" s="105"/>
+      <c r="BB77" s="105"/>
+      <c r="BC77" s="105"/>
+      <c r="BD77" s="105"/>
+      <c r="BE77" s="105"/>
+      <c r="BF77" s="105"/>
+      <c r="BG77" s="105"/>
+      <c r="BH77" s="105"/>
+      <c r="BI77" s="105"/>
+      <c r="BJ77" s="105"/>
+      <c r="BK77" s="105"/>
+      <c r="BL77" s="105"/>
+      <c r="BM77" s="105"/>
+      <c r="BN77" s="105"/>
+    </row>
+    <row r="78" spans="1:66" s="33" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A78" s="30"/>
+      <c r="B78" s="31"/>
+      <c r="C78" s="31"/>
+      <c r="D78" s="32"/>
+      <c r="E78" s="31"/>
+      <c r="F78" s="31"/>
+      <c r="G78" s="31"/>
+      <c r="H78" s="31"/>
+      <c r="I78" s="31"/>
+      <c r="J78" s="31"/>
+      <c r="K78" s="31"/>
+      <c r="L78" s="31"/>
+      <c r="M78" s="31"/>
+      <c r="N78" s="31"/>
+      <c r="O78" s="31"/>
+      <c r="P78" s="31"/>
+      <c r="Q78" s="31"/>
+      <c r="R78" s="31"/>
+      <c r="S78" s="31"/>
+      <c r="T78" s="31"/>
+      <c r="U78" s="31"/>
+      <c r="V78" s="31"/>
+      <c r="W78" s="31"/>
+      <c r="X78" s="31"/>
+      <c r="Y78" s="31"/>
+      <c r="Z78" s="31"/>
+      <c r="AA78" s="31"/>
+      <c r="AB78" s="31"/>
+      <c r="AC78" s="31"/>
+      <c r="AD78" s="31"/>
+      <c r="AE78" s="31"/>
+      <c r="AF78" s="31"/>
+      <c r="AG78" s="31"/>
+      <c r="AH78" s="31"/>
+      <c r="AI78" s="31"/>
+      <c r="AJ78" s="31"/>
+      <c r="AK78" s="31"/>
+      <c r="AL78" s="31"/>
+      <c r="AM78" s="31"/>
+      <c r="AN78" s="31"/>
+      <c r="AO78" s="31"/>
+      <c r="AP78" s="31"/>
+      <c r="AQ78" s="31"/>
+      <c r="AR78" s="31"/>
+      <c r="AS78" s="31"/>
+      <c r="AT78" s="31"/>
+      <c r="AU78" s="31"/>
+      <c r="AV78" s="31"/>
+      <c r="AW78" s="31"/>
+      <c r="AX78" s="31"/>
+      <c r="AY78" s="31"/>
+      <c r="AZ78" s="31"/>
+      <c r="BA78" s="31"/>
+      <c r="BB78" s="31"/>
+      <c r="BC78" s="31"/>
+      <c r="BD78" s="31"/>
+      <c r="BE78" s="31"/>
+      <c r="BF78" s="31"/>
+      <c r="BG78" s="31"/>
+      <c r="BH78" s="31"/>
+      <c r="BI78" s="31"/>
+      <c r="BJ78" s="31"/>
+      <c r="BK78" s="31"/>
+      <c r="BL78" s="31"/>
+      <c r="BM78" s="31"/>
+      <c r="BN78" s="31"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
-    <mergeCell ref="K1:AE1"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="Y4:AE4"/>
-    <mergeCell ref="Y5:AE5"/>
     <mergeCell ref="AF4:AL4"/>
     <mergeCell ref="AF5:AL5"/>
     <mergeCell ref="BH4:BN4"/>
@@ -10403,10 +10962,19 @@
     <mergeCell ref="AM4:AS4"/>
     <mergeCell ref="BA4:BG4"/>
     <mergeCell ref="BA5:BG5"/>
+    <mergeCell ref="K1:AE1"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="R5:X5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="Y4:AE4"/>
+    <mergeCell ref="Y5:AE5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="H8:H11 H16:H18 H66:H72 H30 H20:H28 H13">
-    <cfRule type="dataBar" priority="206">
+  <conditionalFormatting sqref="H8:H11 H16:H18 H71:H77 H30 H20:H28 H13">
+    <cfRule type="dataBar" priority="226">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10420,25 +10988,25 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6:BN7">
-    <cfRule type="expression" dxfId="65" priority="249">
+    <cfRule type="expression" dxfId="80" priority="269">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K8:BN11 K13:BN18 K20:BN30 K33:BN34 K37:BN53 K56:BN72">
-    <cfRule type="expression" dxfId="64" priority="252">
+  <conditionalFormatting sqref="K8:BN11 K13:BN18 K20:BN30 K33:BN34 K37:BN53 K56:BN57 K63:BN77">
+    <cfRule type="expression" dxfId="79" priority="272">
       <formula>AND($E8&lt;=K$6,ROUNDDOWN(($F8-$E8+1)*$H8,0)+$E8-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="253">
+    <cfRule type="expression" dxfId="78" priority="273">
       <formula>AND(NOT(ISBLANK($E8)),$E8&lt;=K$6,$F8&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K6:BN11 K16:BN18 K66:BN72 K30:BN30 K20:BN28 K13:BN13">
-    <cfRule type="expression" dxfId="62" priority="212">
+  <conditionalFormatting sqref="K6:BN11 K16:BN18 K71:BN77 K30:BN30 K20:BN28 K13:BN13">
+    <cfRule type="expression" dxfId="77" priority="232">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15">
-    <cfRule type="dataBar" priority="190">
+    <cfRule type="dataBar" priority="210">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10452,17 +11020,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15:BN15">
-    <cfRule type="expression" dxfId="61" priority="197">
+    <cfRule type="expression" dxfId="76" priority="217">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K14:BN14">
-    <cfRule type="expression" dxfId="60" priority="193">
+    <cfRule type="expression" dxfId="75" priority="213">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H14">
-    <cfRule type="dataBar" priority="191">
+    <cfRule type="dataBar" priority="211">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10476,7 +11044,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33">
-    <cfRule type="dataBar" priority="183">
+    <cfRule type="dataBar" priority="203">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10490,12 +11058,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K33:BN33">
-    <cfRule type="expression" dxfId="59" priority="184">
+    <cfRule type="expression" dxfId="74" priority="204">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H34">
-    <cfRule type="dataBar" priority="175">
+    <cfRule type="dataBar" priority="195">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10509,7 +11077,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H40">
-    <cfRule type="dataBar" priority="167">
+    <cfRule type="dataBar" priority="187">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10523,12 +11091,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K34:BN34">
-    <cfRule type="expression" dxfId="58" priority="176">
+    <cfRule type="expression" dxfId="73" priority="196">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H57">
-    <cfRule type="dataBar" priority="159">
+    <cfRule type="dataBar" priority="179">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10542,12 +11110,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K40:BN40">
-    <cfRule type="expression" dxfId="57" priority="168">
+    <cfRule type="expression" dxfId="72" priority="188">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H39">
-    <cfRule type="dataBar" priority="171">
+    <cfRule type="dataBar" priority="191">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10561,12 +11129,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K39:BN39">
-    <cfRule type="expression" dxfId="56" priority="172">
+    <cfRule type="expression" dxfId="71" priority="192">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H65">
-    <cfRule type="dataBar" priority="151">
+  <conditionalFormatting sqref="H70">
+    <cfRule type="dataBar" priority="171">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10580,12 +11148,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K57:BN57">
-    <cfRule type="expression" dxfId="55" priority="160">
+    <cfRule type="expression" dxfId="70" priority="180">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H61">
-    <cfRule type="dataBar" priority="143">
+  <conditionalFormatting sqref="H66">
+    <cfRule type="dataBar" priority="163">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10598,13 +11166,13 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K65:BN65">
-    <cfRule type="expression" dxfId="54" priority="152">
+  <conditionalFormatting sqref="K70:BN70">
+    <cfRule type="expression" dxfId="69" priority="172">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H56">
-    <cfRule type="dataBar" priority="163">
+    <cfRule type="dataBar" priority="183">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10618,12 +11186,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K56:BN56">
-    <cfRule type="expression" dxfId="53" priority="164">
+    <cfRule type="expression" dxfId="68" priority="184">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H59">
-    <cfRule type="dataBar" priority="135">
+  <conditionalFormatting sqref="H64">
+    <cfRule type="dataBar" priority="155">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10636,13 +11204,13 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K61:BN61">
-    <cfRule type="expression" dxfId="52" priority="144">
+  <conditionalFormatting sqref="K66:BN66">
+    <cfRule type="expression" dxfId="67" priority="164">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H64">
-    <cfRule type="dataBar" priority="155">
+  <conditionalFormatting sqref="H69">
+    <cfRule type="dataBar" priority="175">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10655,13 +11223,13 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K64:BN64">
-    <cfRule type="expression" dxfId="51" priority="156">
+  <conditionalFormatting sqref="K69:BN69">
+    <cfRule type="expression" dxfId="66" priority="176">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H45">
-    <cfRule type="dataBar" priority="127">
+    <cfRule type="dataBar" priority="147">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10674,13 +11242,13 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K59:BN59">
-    <cfRule type="expression" dxfId="50" priority="136">
+  <conditionalFormatting sqref="K64:BN64">
+    <cfRule type="expression" dxfId="65" priority="156">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H60">
-    <cfRule type="dataBar" priority="147">
+  <conditionalFormatting sqref="H65">
+    <cfRule type="dataBar" priority="167">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10693,13 +11261,13 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K60:BN60">
-    <cfRule type="expression" dxfId="49" priority="148">
+  <conditionalFormatting sqref="K65:BN65">
+    <cfRule type="expression" dxfId="64" priority="168">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H43">
-    <cfRule type="dataBar" priority="119">
+    <cfRule type="dataBar" priority="139">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10713,12 +11281,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K45:BN45">
-    <cfRule type="expression" dxfId="48" priority="128">
+    <cfRule type="expression" dxfId="63" priority="148">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H58">
-    <cfRule type="dataBar" priority="139">
+  <conditionalFormatting sqref="H63">
+    <cfRule type="dataBar" priority="159">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10731,13 +11299,13 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K58:BN58">
-    <cfRule type="expression" dxfId="47" priority="140">
+  <conditionalFormatting sqref="K63:BN63">
+    <cfRule type="expression" dxfId="62" priority="160">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H63">
-    <cfRule type="dataBar" priority="111">
+  <conditionalFormatting sqref="H68">
+    <cfRule type="dataBar" priority="131">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10751,12 +11319,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K43:BN43">
-    <cfRule type="expression" dxfId="46" priority="120">
+    <cfRule type="expression" dxfId="61" priority="140">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H44">
-    <cfRule type="dataBar" priority="131">
+    <cfRule type="dataBar" priority="151">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10770,12 +11338,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K44:BN44">
-    <cfRule type="expression" dxfId="45" priority="132">
+    <cfRule type="expression" dxfId="60" priority="152">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29">
-    <cfRule type="dataBar" priority="107">
+    <cfRule type="dataBar" priority="127">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10788,13 +11356,13 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K63:BN63">
-    <cfRule type="expression" dxfId="44" priority="112">
+  <conditionalFormatting sqref="K68:BN68">
+    <cfRule type="expression" dxfId="59" priority="132">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H41">
-    <cfRule type="dataBar" priority="123">
+    <cfRule type="dataBar" priority="143">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10808,17 +11376,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K41:BN41">
-    <cfRule type="expression" dxfId="43" priority="124">
+    <cfRule type="expression" dxfId="58" priority="144">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K29:BN29">
-    <cfRule type="expression" dxfId="42" priority="108">
+    <cfRule type="expression" dxfId="57" priority="128">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H62">
-    <cfRule type="dataBar" priority="115">
+  <conditionalFormatting sqref="H67">
+    <cfRule type="dataBar" priority="135">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10831,13 +11399,13 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K62:BN62">
-    <cfRule type="expression" dxfId="41" priority="116">
+  <conditionalFormatting sqref="K67:BN67">
+    <cfRule type="expression" dxfId="56" priority="136">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12">
-    <cfRule type="dataBar" priority="89">
+    <cfRule type="dataBar" priority="109">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10851,20 +11419,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12:BN12">
-    <cfRule type="expression" dxfId="40" priority="91">
+    <cfRule type="expression" dxfId="55" priority="111">
       <formula>AND($E12&lt;=K$6,ROUNDDOWN(($F12-$E12+1)*$H12,0)+$E12-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="92">
+    <cfRule type="expression" dxfId="54" priority="112">
       <formula>AND(NOT(ISBLANK($E12)),$E12&lt;=K$6,$F12&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12:BN12">
-    <cfRule type="expression" dxfId="38" priority="90">
+    <cfRule type="expression" dxfId="53" priority="110">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H19">
-    <cfRule type="dataBar" priority="85">
+    <cfRule type="dataBar" priority="105">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10878,20 +11446,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K19:BN19">
-    <cfRule type="expression" dxfId="37" priority="87">
+    <cfRule type="expression" dxfId="52" priority="107">
       <formula>AND($E19&lt;=K$6,ROUNDDOWN(($F19-$E19+1)*$H19,0)+$E19-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="88">
+    <cfRule type="expression" dxfId="51" priority="108">
       <formula>AND(NOT(ISBLANK($E19)),$E19&lt;=K$6,$F19&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K19:BN19">
-    <cfRule type="expression" dxfId="35" priority="86">
+    <cfRule type="expression" dxfId="50" priority="106">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H31">
-    <cfRule type="dataBar" priority="81">
+    <cfRule type="dataBar" priority="101">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10905,20 +11473,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K31:BN31">
-    <cfRule type="expression" dxfId="34" priority="83">
+    <cfRule type="expression" dxfId="49" priority="103">
       <formula>AND($E31&lt;=K$6,ROUNDDOWN(($F31-$E31+1)*$H31,0)+$E31-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="84">
+    <cfRule type="expression" dxfId="48" priority="104">
       <formula>AND(NOT(ISBLANK($E31)),$E31&lt;=K$6,$F31&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K31:BN31">
-    <cfRule type="expression" dxfId="32" priority="82">
+    <cfRule type="expression" dxfId="47" priority="102">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H42">
-    <cfRule type="dataBar" priority="77">
+    <cfRule type="dataBar" priority="97">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10932,12 +11500,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K42:BN42">
-    <cfRule type="expression" dxfId="31" priority="78">
+    <cfRule type="expression" dxfId="46" priority="98">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H44">
-    <cfRule type="dataBar" priority="75">
+    <cfRule type="dataBar" priority="95">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10951,12 +11519,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K44:BN44">
-    <cfRule type="expression" dxfId="30" priority="76">
+    <cfRule type="expression" dxfId="45" priority="96">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H43">
-    <cfRule type="dataBar" priority="71">
+    <cfRule type="dataBar" priority="91">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10970,12 +11538,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K43:BN43">
-    <cfRule type="expression" dxfId="29" priority="72">
+    <cfRule type="expression" dxfId="44" priority="92">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H49">
-    <cfRule type="dataBar" priority="65">
+    <cfRule type="dataBar" priority="85">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10989,7 +11557,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H47">
-    <cfRule type="dataBar" priority="63">
+    <cfRule type="dataBar" priority="83">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -11003,17 +11571,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K49:BN49">
-    <cfRule type="expression" dxfId="28" priority="66">
+    <cfRule type="expression" dxfId="43" priority="86">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K47:BN47">
-    <cfRule type="expression" dxfId="27" priority="64">
+    <cfRule type="expression" dxfId="42" priority="84">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H48">
-    <cfRule type="dataBar" priority="67">
+    <cfRule type="dataBar" priority="87">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -11027,12 +11595,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K48:BN48">
-    <cfRule type="expression" dxfId="26" priority="68">
+    <cfRule type="expression" dxfId="41" priority="88">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H46">
-    <cfRule type="dataBar" priority="59">
+    <cfRule type="dataBar" priority="79">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -11046,12 +11614,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K46:BN46">
-    <cfRule type="expression" dxfId="25" priority="60">
+    <cfRule type="expression" dxfId="40" priority="80">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H48">
-    <cfRule type="dataBar" priority="57">
+    <cfRule type="dataBar" priority="77">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -11065,12 +11633,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K48:BN48">
-    <cfRule type="expression" dxfId="24" priority="58">
+    <cfRule type="expression" dxfId="39" priority="78">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H47">
-    <cfRule type="dataBar" priority="53">
+    <cfRule type="dataBar" priority="73">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -11084,12 +11652,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K47:BN47">
-    <cfRule type="expression" dxfId="23" priority="54">
+    <cfRule type="expression" dxfId="38" priority="74">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H51">
-    <cfRule type="dataBar" priority="47">
+    <cfRule type="dataBar" priority="67">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -11103,12 +11671,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K51:BN51">
-    <cfRule type="expression" dxfId="22" priority="48">
+    <cfRule type="expression" dxfId="37" priority="68">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H52">
-    <cfRule type="dataBar" priority="49">
+    <cfRule type="dataBar" priority="69">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -11122,12 +11690,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K52:BN52">
-    <cfRule type="expression" dxfId="21" priority="50">
+    <cfRule type="expression" dxfId="36" priority="70">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H50">
-    <cfRule type="dataBar" priority="43">
+    <cfRule type="dataBar" priority="63">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -11141,12 +11709,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K50:BN50">
-    <cfRule type="expression" dxfId="20" priority="44">
+    <cfRule type="expression" dxfId="35" priority="64">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H52">
-    <cfRule type="dataBar" priority="41">
+    <cfRule type="dataBar" priority="61">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -11160,12 +11728,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K52:BN52">
-    <cfRule type="expression" dxfId="19" priority="42">
+    <cfRule type="expression" dxfId="34" priority="62">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H51">
-    <cfRule type="dataBar" priority="37">
+    <cfRule type="dataBar" priority="57">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -11179,12 +11747,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K51:BN51">
-    <cfRule type="expression" dxfId="18" priority="38">
+    <cfRule type="expression" dxfId="33" priority="58">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32">
-    <cfRule type="dataBar" priority="33">
+    <cfRule type="dataBar" priority="53">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -11198,28 +11766,28 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32:BN32">
-    <cfRule type="expression" dxfId="17" priority="35">
+    <cfRule type="expression" dxfId="32" priority="55">
       <formula>AND($E32&lt;=K$6,ROUNDDOWN(($F32-$E32+1)*$H32,0)+$E32-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="36">
+    <cfRule type="expression" dxfId="31" priority="56">
       <formula>AND(NOT(ISBLANK($E32)),$E32&lt;=K$6,$F32&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32:BN32">
-    <cfRule type="expression" dxfId="15" priority="34">
+    <cfRule type="expression" dxfId="30" priority="54">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K35:BN35">
-    <cfRule type="expression" dxfId="14" priority="31">
+    <cfRule type="expression" dxfId="29" priority="51">
       <formula>AND($E35&lt;=K$6,ROUNDDOWN(($F35-$E35+1)*$H35,0)+$E35-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="32">
+    <cfRule type="expression" dxfId="28" priority="52">
       <formula>AND(NOT(ISBLANK($E35)),$E35&lt;=K$6,$F35&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H35">
-    <cfRule type="dataBar" priority="29">
+    <cfRule type="dataBar" priority="49">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -11233,20 +11801,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K35:BN35">
-    <cfRule type="expression" dxfId="12" priority="30">
+    <cfRule type="expression" dxfId="27" priority="50">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K36:BN36">
-    <cfRule type="expression" dxfId="11" priority="27">
+    <cfRule type="expression" dxfId="26" priority="47">
       <formula>AND($E36&lt;=K$6,ROUNDDOWN(($F36-$E36+1)*$H36,0)+$E36-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="28">
+    <cfRule type="expression" dxfId="25" priority="48">
       <formula>AND(NOT(ISBLANK($E36)),$E36&lt;=K$6,$F36&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H36">
-    <cfRule type="dataBar" priority="25">
+    <cfRule type="dataBar" priority="45">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -11260,12 +11828,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K36:BN36">
-    <cfRule type="expression" dxfId="9" priority="26">
+    <cfRule type="expression" dxfId="24" priority="46">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H37">
-    <cfRule type="dataBar" priority="17">
+    <cfRule type="dataBar" priority="37">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -11279,12 +11847,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K37:BN37">
-    <cfRule type="expression" dxfId="8" priority="18">
+    <cfRule type="expression" dxfId="23" priority="38">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H38">
-    <cfRule type="dataBar" priority="13">
+    <cfRule type="dataBar" priority="33">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -11298,12 +11866,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K38:BN38">
-    <cfRule type="expression" dxfId="7" priority="14">
+    <cfRule type="expression" dxfId="22" priority="34">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H53">
-    <cfRule type="dataBar" priority="9">
+    <cfRule type="dataBar" priority="29">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -11317,12 +11885,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K53:BN53">
-    <cfRule type="expression" dxfId="6" priority="10">
+    <cfRule type="expression" dxfId="21" priority="30">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H54">
-    <cfRule type="dataBar" priority="5">
+    <cfRule type="dataBar" priority="25">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -11336,20 +11904,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K54:BN54">
-    <cfRule type="expression" dxfId="5" priority="7">
+    <cfRule type="expression" dxfId="20" priority="27">
       <formula>AND($E54&lt;=K$6,ROUNDDOWN(($F54-$E54+1)*$H54,0)+$E54-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="8">
+    <cfRule type="expression" dxfId="19" priority="28">
       <formula>AND(NOT(ISBLANK($E54)),$E54&lt;=K$6,$F54&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K54:BN54">
-    <cfRule type="expression" dxfId="3" priority="6">
+    <cfRule type="expression" dxfId="18" priority="26">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H55">
-    <cfRule type="dataBar" priority="1">
+    <cfRule type="dataBar" priority="21">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -11363,27 +11931,162 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K55:BN55">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="17" priority="23">
       <formula>AND($E55&lt;=K$6,ROUNDDOWN(($F55-$E55+1)*$H55,0)+$E55-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="4">
+    <cfRule type="expression" dxfId="16" priority="24">
       <formula>AND(NOT(ISBLANK($E55)),$E55&lt;=K$6,$F55&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K55:BN55">
+    <cfRule type="expression" dxfId="15" priority="22">
+      <formula>K$6=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K59:BN59">
+    <cfRule type="expression" dxfId="14" priority="19">
+      <formula>AND($E59&lt;=K$6,ROUNDDOWN(($F59-$E59+1)*$H59,0)+$E59-1&gt;=K$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="20">
+      <formula>AND(NOT(ISBLANK($E59)),$E59&lt;=K$6,$F59&gt;=K$6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H59">
+    <cfRule type="dataBar" priority="17">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{6A660D63-3B7F-A749-B18A-47D5F4FD4BD3}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K59:BN59">
+    <cfRule type="expression" dxfId="12" priority="18">
+      <formula>K$6=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K60:BN60">
+    <cfRule type="expression" dxfId="11" priority="15">
+      <formula>AND($E60&lt;=K$6,ROUNDDOWN(($F60-$E60+1)*$H60,0)+$E60-1&gt;=K$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="16">
+      <formula>AND(NOT(ISBLANK($E60)),$E60&lt;=K$6,$F60&gt;=K$6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H60">
+    <cfRule type="dataBar" priority="13">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{06AA0FD3-EBB4-C646-9DA4-4C52010BF18E}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K60:BN60">
+    <cfRule type="expression" dxfId="9" priority="14">
+      <formula>K$6=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K58:BN58">
+    <cfRule type="expression" dxfId="8" priority="11">
+      <formula>AND($E58&lt;=K$6,ROUNDDOWN(($F58-$E58+1)*$H58,0)+$E58-1&gt;=K$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="12">
+      <formula>AND(NOT(ISBLANK($E58)),$E58&lt;=K$6,$F58&gt;=K$6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H58">
+    <cfRule type="dataBar" priority="9">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{EA0F6348-41A2-2C4E-AF86-40C164BC7828}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K58:BN58">
+    <cfRule type="expression" dxfId="6" priority="10">
+      <formula>K$6=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K62:BN62">
+    <cfRule type="expression" dxfId="5" priority="7">
+      <formula>AND($E62&lt;=K$6,ROUNDDOWN(($F62-$E62+1)*$H62,0)+$E62-1&gt;=K$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="8">
+      <formula>AND(NOT(ISBLANK($E62)),$E62&lt;=K$6,$F62&gt;=K$6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H62">
+    <cfRule type="dataBar" priority="5">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{F8A8856B-52A6-514C-B303-65920B23BA6E}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K62:BN62">
+    <cfRule type="expression" dxfId="3" priority="6">
+      <formula>K$6=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K61:BN61">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>AND($E61&lt;=K$6,ROUNDDOWN(($F61-$E61+1)*$H61,0)+$E61-1&gt;=K$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="4">
+      <formula>AND(NOT(ISBLANK($E61)),$E61&lt;=K$6,$F61&gt;=K$6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H61">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{D1A71D1C-EF1B-8540-A82B-798D6780A3B4}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K61:BN61">
     <cfRule type="expression" dxfId="0" priority="2">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Display Week" prompt="Enter the week number to display first in the Gantt Chart. The weeks are numbered starting from the week containing the Project Start Date." sqref="H4"/>
   </dataValidations>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.5" footer="0.25"/>
   <pageSetup scale="55" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <ignoredErrors>
-    <ignoredError sqref="A66:B66 A68:B68 B67 E10 E20 E24 E66:H68 G10:H10 G20:H20 G24:H24 G69 G70:G71 G72 G25" unlockedFormula="1"/>
-    <ignoredError sqref="A24 A20 A10 A16 A54 A56 A58 A60 A62 A64" formula="1"/>
+    <ignoredError sqref="A71:B71 A73:B73 B72 E10 E20 E24 E71:H73 G10:H10 G20:H20 G24:H24 G74 G75:G76 G77 G25" unlockedFormula="1"/>
+    <ignoredError sqref="A24 A20 A10 A16 A54 A56 A63 A65 A67 A69" formula="1"/>
   </ignoredErrors>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
@@ -11433,7 +12136,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H8:H11 H16:H18 H66:H72 H30 H20:H28 H13</xm:sqref>
+          <xm:sqref>H8:H11 H16:H18 H71:H77 H30 H20:H28 H13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{C1E55C9C-328E-7F42-B324-A31B3CE69B6E}">
@@ -11553,7 +12256,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H65</xm:sqref>
+          <xm:sqref>H70</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{F222E3D4-7513-264C-968B-0292F382CD5D}">
@@ -11568,7 +12271,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H61</xm:sqref>
+          <xm:sqref>H66</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{526828FD-A928-6E46-95F8-D74ACD1E339B}">
@@ -11598,7 +12301,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H59</xm:sqref>
+          <xm:sqref>H64</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{1C2DB213-53A8-4946-B60A-C01681F15068}">
@@ -11613,7 +12316,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H64</xm:sqref>
+          <xm:sqref>H69</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{D8388F22-1F90-F24E-9C6B-625491BBF15E}">
@@ -11643,7 +12346,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H60</xm:sqref>
+          <xm:sqref>H65</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{6CC7F112-D4C4-2647-8F58-25080F8D0653}">
@@ -11673,7 +12376,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H58</xm:sqref>
+          <xm:sqref>H63</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{A44EC134-680C-6943-A530-937463E3A665}">
@@ -11688,7 +12391,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H63</xm:sqref>
+          <xm:sqref>H68</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{6900B624-12B9-8C44-99D7-233CE13C7600}">
@@ -11748,7 +12451,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H62</xm:sqref>
+          <xm:sqref>H67</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{B72F9582-8103-A840-9EC3-CEB5270C8B2A}">
@@ -12125,6 +12828,81 @@
           </x14:cfRule>
           <xm:sqref>H55</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{6A660D63-3B7F-A749-B18A-47D5F4FD4BD3}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H59</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{06AA0FD3-EBB4-C646-9DA4-4C52010BF18E}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H60</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{EA0F6348-41A2-2C4E-AF86-40C164BC7828}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H58</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{F8A8856B-52A6-514C-B303-65920B23BA6E}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H62</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{D1A71D1C-EF1B-8540-A82B-798D6780A3B4}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H61</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>

</xml_diff>